<commit_message>
Aggiunte analisi CodeT5_770, aggiunta creazione grafico per distribuzione common failure, aggiunto il requisito matplotlib
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/Analisi_CodeT5_770.xlsx
+++ b/HE/W_in_progress/Analisi_CodeT5_770.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28312"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C52276ED-5378-4504-8980-8920AE72827E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81B46834-1967-40AD-AD3A-13FAE31FCD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="1116">
   <si>
     <t>IN</t>
   </si>
@@ -2166,6 +2166,9 @@
     <t>0.619047614058957</t>
   </si>
   <si>
+    <t>Qualche problemino vma va bene</t>
+  </si>
+  <si>
     <t>Define a frequency divider with the signals clock, reset, and divide_ratio (N-bit) as input and the signal divided_clock as output.</t>
   </si>
   <si>
@@ -2181,6 +2184,9 @@
     <t>0.8421052581717452</t>
   </si>
   <si>
+    <t>E' un divisore di frequenza</t>
+  </si>
+  <si>
     <t>Create a basic SPI (Serial Peripheral Interface) master with multiple slave select</t>
   </si>
   <si>
@@ -2196,6 +2202,9 @@
     <t>0.33333332897764634</t>
   </si>
   <si>
+    <t>Non proprio un master SPI</t>
+  </si>
+  <si>
     <t>Create a basic PWM (Pulse Width Modulation) generator with variable frequency</t>
   </si>
   <si>
@@ -2286,6 +2295,9 @@
     <t>0.366197178385241</t>
   </si>
   <si>
+    <t>Completamente un altra cosa</t>
+  </si>
+  <si>
     <t>Define a debouncer with the signal noisy_button as input and the signal clean_button_pulse as output.</t>
   </si>
   <si>
@@ -2301,6 +2313,9 @@
     <t>0.6981132025631898</t>
   </si>
   <si>
+    <t>Debouncer semplice, ma è un dbouncer</t>
+  </si>
+  <si>
     <t>Define a Johnson ring counter of N-bit with the signals clock and reset as input and the signal count (N-bit) as output.</t>
   </si>
   <si>
@@ -2331,6 +2346,9 @@
     <t>0.7787610569472943</t>
   </si>
   <si>
+    <t>Non genera un impulso</t>
+  </si>
+  <si>
     <t>Define a magnitude comparator of K-bit with the signals A (K-bit) and B (K-bit) as input and the signals A_GT_B, A_EQ_B, and A_LT_B as output.</t>
   </si>
   <si>
@@ -2344,6 +2362,9 @@
   </si>
   <si>
     <t>0.7961164998586108</t>
+  </si>
+  <si>
+    <t>Il confronto non va bene</t>
   </si>
   <si>
     <t>Define a pseudo-random number generator of N-bit with the signals clock and seed_value (N-bit) as input and the signal random_number (N-bit) as output.</t>
@@ -3731,7 +3752,7 @@
   <dimension ref="A1:L327"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="L231" sqref="L231"/>
+      <selection activeCell="C249" sqref="C249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11916,7 +11937,7 @@
         <v>700</v>
       </c>
       <c r="K231">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:12">
@@ -11951,7 +11972,7 @@
         <v>705</v>
       </c>
       <c r="K232">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:12">
@@ -11986,18 +12007,21 @@
         <v>710</v>
       </c>
       <c r="K233">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L233" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="234" spans="1:12">
       <c r="A234" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B234" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C234" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D234">
         <v>0</v>
@@ -12009,7 +12033,7 @@
         <v>0.62843943725002704</v>
       </c>
       <c r="G234" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="H234">
         <v>0.52</v>
@@ -12018,21 +12042,24 @@
         <v>0.93110000000000004</v>
       </c>
       <c r="J234" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="K234">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L234" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="235" spans="1:12">
       <c r="A235" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B235" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C235" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="D235">
         <v>0</v>
@@ -12044,7 +12071,7 @@
         <v>0.25705627789553498</v>
       </c>
       <c r="G235" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="H235">
         <v>0.02</v>
@@ -12053,21 +12080,24 @@
         <v>0.6762999999999999</v>
       </c>
       <c r="J235" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="K235">
         <v>0</v>
+      </c>
+      <c r="L235" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="236" spans="1:12">
       <c r="A236" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B236" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C236" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="D236">
         <v>0</v>
@@ -12079,7 +12109,7 @@
         <v>0.78236533442344558</v>
       </c>
       <c r="G236" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="H236">
         <v>0.16</v>
@@ -12088,21 +12118,21 @@
         <v>0.64870000000000005</v>
       </c>
       <c r="J236" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="K236">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:12">
       <c r="A237" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="B237" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="C237" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -12114,7 +12144,7 @@
         <v>0.52692313644855682</v>
       </c>
       <c r="G237" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="H237">
         <v>0.31</v>
@@ -12123,21 +12153,21 @@
         <v>0.8276</v>
       </c>
       <c r="J237" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="K237">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:12">
       <c r="A238" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="B238" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="C238" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -12149,7 +12179,7 @@
         <v>0.57456483731345098</v>
       </c>
       <c r="G238" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="H238">
         <v>0.36</v>
@@ -12158,21 +12188,21 @@
         <v>0.91830000000000001</v>
       </c>
       <c r="J238" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="K238">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:12">
       <c r="A239" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="B239" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="C239" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -12184,7 +12214,7 @@
         <v>0.32783920985556497</v>
       </c>
       <c r="G239" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="H239">
         <v>0.18</v>
@@ -12193,21 +12223,21 @@
         <v>0.82310000000000005</v>
       </c>
       <c r="J239" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="K239">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:12">
       <c r="A240" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="B240" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="C240" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="D240">
         <v>0</v>
@@ -12219,7 +12249,7 @@
         <v>0.74029969876453894</v>
       </c>
       <c r="G240" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="H240">
         <v>0.39</v>
@@ -12228,21 +12258,24 @@
         <v>0.84340000000000004</v>
       </c>
       <c r="J240" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="K240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:11">
+      <c r="L240" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12">
       <c r="A241" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="B241" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="C241" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -12254,7 +12287,7 @@
         <v>0.36345675793343268</v>
       </c>
       <c r="G241" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="H241">
         <v>0</v>
@@ -12263,21 +12296,24 @@
         <v>0.36159999999999998</v>
       </c>
       <c r="J241" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="K241">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:11">
+      <c r="L241" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12">
       <c r="A242" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="B242" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="C242" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="D242">
         <v>0</v>
@@ -12289,7 +12325,7 @@
         <v>0.48098435430025749</v>
       </c>
       <c r="G242" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="H242">
         <v>0.28999999999999998</v>
@@ -12298,21 +12334,24 @@
         <v>0.84079999999999999</v>
       </c>
       <c r="J242" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="K242">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L242" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12">
       <c r="A243" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="B243" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
       <c r="C243" t="s">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -12324,7 +12363,7 @@
         <v>0.91703151395258087</v>
       </c>
       <c r="G243" t="s">
-        <v>759</v>
+        <v>764</v>
       </c>
       <c r="H243">
         <v>0.48</v>
@@ -12333,21 +12372,21 @@
         <v>0.85699999999999998</v>
       </c>
       <c r="J243" t="s">
-        <v>760</v>
+        <v>765</v>
       </c>
       <c r="K243">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12">
       <c r="A244" t="s">
-        <v>761</v>
+        <v>766</v>
       </c>
       <c r="B244" t="s">
-        <v>762</v>
+        <v>767</v>
       </c>
       <c r="C244" t="s">
-        <v>763</v>
+        <v>768</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -12359,7 +12398,7 @@
         <v>0.54712326151393509</v>
       </c>
       <c r="G244" t="s">
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="H244">
         <v>0.44</v>
@@ -12368,21 +12407,24 @@
         <v>0.97659999999999991</v>
       </c>
       <c r="J244" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
       <c r="K244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:11">
+      <c r="L244" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12">
       <c r="A245" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="B245" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="C245" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -12394,7 +12436,7 @@
         <v>0.50184113064577929</v>
       </c>
       <c r="G245" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="H245">
         <v>0.57999999999999996</v>
@@ -12403,21 +12445,24 @@
         <v>0.90180000000000005</v>
       </c>
       <c r="J245" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="K245">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:11">
+      <c r="L245" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12">
       <c r="A246" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
       <c r="B246" t="s">
-        <v>772</v>
+        <v>779</v>
       </c>
       <c r="C246" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -12429,7 +12474,7 @@
         <v>0.53141508942106874</v>
       </c>
       <c r="G246" t="s">
-        <v>774</v>
+        <v>781</v>
       </c>
       <c r="H246">
         <v>0.11</v>
@@ -12438,21 +12483,21 @@
         <v>0.78139999999999998</v>
       </c>
       <c r="J246" t="s">
-        <v>775</v>
+        <v>782</v>
       </c>
       <c r="K246">
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:12">
       <c r="A247" t="s">
-        <v>776</v>
+        <v>783</v>
       </c>
       <c r="B247" t="s">
-        <v>777</v>
+        <v>784</v>
       </c>
       <c r="C247" t="s">
-        <v>778</v>
+        <v>785</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -12464,7 +12509,7 @@
         <v>0.51524183187482964</v>
       </c>
       <c r="G247" t="s">
-        <v>779</v>
+        <v>786</v>
       </c>
       <c r="H247">
         <v>0.24</v>
@@ -12479,15 +12524,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:12">
       <c r="A248" t="s">
-        <v>780</v>
+        <v>787</v>
       </c>
       <c r="B248" t="s">
-        <v>781</v>
+        <v>788</v>
       </c>
       <c r="C248" t="s">
-        <v>782</v>
+        <v>789</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -12499,7 +12544,7 @@
         <v>0.78286006472129221</v>
       </c>
       <c r="G248" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
       <c r="H248">
         <v>0.31</v>
@@ -12508,21 +12553,21 @@
         <v>0.875</v>
       </c>
       <c r="J248" t="s">
-        <v>784</v>
+        <v>791</v>
       </c>
       <c r="K248">
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:12">
       <c r="A249" t="s">
-        <v>785</v>
+        <v>792</v>
       </c>
       <c r="B249" t="s">
-        <v>786</v>
+        <v>793</v>
       </c>
       <c r="C249" t="s">
-        <v>787</v>
+        <v>794</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -12534,7 +12579,7 @@
         <v>0.70670746171322651</v>
       </c>
       <c r="G249" t="s">
-        <v>788</v>
+        <v>795</v>
       </c>
       <c r="H249">
         <v>0.56999999999999995</v>
@@ -12543,21 +12588,21 @@
         <v>0.83079999999999998</v>
       </c>
       <c r="J249" t="s">
-        <v>789</v>
+        <v>796</v>
       </c>
       <c r="K249">
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:12">
       <c r="A250" t="s">
-        <v>790</v>
+        <v>797</v>
       </c>
       <c r="B250" t="s">
-        <v>791</v>
+        <v>798</v>
       </c>
       <c r="C250" t="s">
-        <v>792</v>
+        <v>799</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -12569,7 +12614,7 @@
         <v>0.55878820772884119</v>
       </c>
       <c r="G250" t="s">
-        <v>793</v>
+        <v>800</v>
       </c>
       <c r="H250">
         <v>0.38</v>
@@ -12578,21 +12623,21 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="J250" t="s">
-        <v>794</v>
+        <v>801</v>
       </c>
       <c r="K250">
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:11">
+    <row r="251" spans="1:12">
       <c r="A251" t="s">
-        <v>795</v>
+        <v>802</v>
       </c>
       <c r="B251" t="s">
-        <v>796</v>
+        <v>803</v>
       </c>
       <c r="C251" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -12604,7 +12649,7 @@
         <v>0.50052628839754476</v>
       </c>
       <c r="G251" t="s">
-        <v>798</v>
+        <v>805</v>
       </c>
       <c r="H251">
         <v>0.42</v>
@@ -12613,21 +12658,21 @@
         <v>0.87659999999999993</v>
       </c>
       <c r="J251" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
       <c r="K251">
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:11">
+    <row r="252" spans="1:12">
       <c r="A252" t="s">
-        <v>800</v>
+        <v>807</v>
       </c>
       <c r="B252" t="s">
-        <v>801</v>
+        <v>808</v>
       </c>
       <c r="C252" t="s">
-        <v>802</v>
+        <v>809</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -12639,7 +12684,7 @@
         <v>0.67954376611458289</v>
       </c>
       <c r="G252" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="H252">
         <v>0.5</v>
@@ -12648,21 +12693,21 @@
         <v>0.7722</v>
       </c>
       <c r="J252" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
       <c r="K252">
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:11">
+    <row r="253" spans="1:12">
       <c r="A253" t="s">
-        <v>805</v>
+        <v>812</v>
       </c>
       <c r="B253" t="s">
-        <v>806</v>
+        <v>813</v>
       </c>
       <c r="C253" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -12674,7 +12719,7 @@
         <v>0.26743188647338118</v>
       </c>
       <c r="G253" t="s">
-        <v>808</v>
+        <v>815</v>
       </c>
       <c r="H253">
         <v>0</v>
@@ -12683,21 +12728,21 @@
         <v>0.84050000000000002</v>
       </c>
       <c r="J253" t="s">
-        <v>809</v>
+        <v>816</v>
       </c>
       <c r="K253">
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:11">
+    <row r="254" spans="1:12">
       <c r="A254" t="s">
-        <v>810</v>
+        <v>817</v>
       </c>
       <c r="B254" t="s">
-        <v>811</v>
+        <v>818</v>
       </c>
       <c r="C254" t="s">
-        <v>812</v>
+        <v>819</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -12709,7 +12754,7 @@
         <v>0.61614612178272654</v>
       </c>
       <c r="G254" t="s">
-        <v>813</v>
+        <v>820</v>
       </c>
       <c r="H254">
         <v>0</v>
@@ -12718,21 +12763,21 @@
         <v>0.82230000000000003</v>
       </c>
       <c r="J254" t="s">
-        <v>814</v>
+        <v>821</v>
       </c>
       <c r="K254">
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:11">
+    <row r="255" spans="1:12">
       <c r="A255" t="s">
-        <v>815</v>
+        <v>822</v>
       </c>
       <c r="B255" t="s">
-        <v>816</v>
+        <v>823</v>
       </c>
       <c r="C255" t="s">
-        <v>817</v>
+        <v>824</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -12744,7 +12789,7 @@
         <v>0.81386184861469513</v>
       </c>
       <c r="G255" t="s">
-        <v>818</v>
+        <v>825</v>
       </c>
       <c r="H255">
         <v>0.67</v>
@@ -12753,21 +12798,21 @@
         <v>0.87769999999999992</v>
       </c>
       <c r="J255" t="s">
-        <v>819</v>
+        <v>826</v>
       </c>
       <c r="K255">
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:11">
+    <row r="256" spans="1:12">
       <c r="A256" t="s">
-        <v>820</v>
+        <v>827</v>
       </c>
       <c r="B256" t="s">
-        <v>821</v>
+        <v>828</v>
       </c>
       <c r="C256" t="s">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -12779,7 +12824,7 @@
         <v>0.34146754595961881</v>
       </c>
       <c r="G256" t="s">
-        <v>823</v>
+        <v>830</v>
       </c>
       <c r="H256">
         <v>0.05</v>
@@ -12788,7 +12833,7 @@
         <v>0.89029999999999998</v>
       </c>
       <c r="J256" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="K256">
         <v>0</v>
@@ -12796,13 +12841,13 @@
     </row>
     <row r="257" spans="1:11">
       <c r="A257" t="s">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c r="B257" t="s">
-        <v>826</v>
+        <v>833</v>
       </c>
       <c r="C257" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -12814,7 +12859,7 @@
         <v>0.52996093454314475</v>
       </c>
       <c r="G257" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="H257">
         <v>0</v>
@@ -12823,7 +12868,7 @@
         <v>0.86849999999999994</v>
       </c>
       <c r="J257" t="s">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c r="K257">
         <v>0</v>
@@ -12831,13 +12876,13 @@
     </row>
     <row r="258" spans="1:11">
       <c r="A258" t="s">
-        <v>830</v>
+        <v>837</v>
       </c>
       <c r="B258" t="s">
-        <v>831</v>
+        <v>838</v>
       </c>
       <c r="C258" t="s">
-        <v>832</v>
+        <v>839</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -12849,7 +12894,7 @@
         <v>0.33777001839693588</v>
       </c>
       <c r="G258" t="s">
-        <v>833</v>
+        <v>840</v>
       </c>
       <c r="H258">
         <v>0.11</v>
@@ -12858,7 +12903,7 @@
         <v>0.87250000000000005</v>
       </c>
       <c r="J258" t="s">
-        <v>834</v>
+        <v>841</v>
       </c>
       <c r="K258">
         <v>0</v>
@@ -12866,13 +12911,13 @@
     </row>
     <row r="259" spans="1:11">
       <c r="A259" t="s">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="B259" t="s">
-        <v>836</v>
+        <v>843</v>
       </c>
       <c r="C259" t="s">
-        <v>837</v>
+        <v>844</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -12884,7 +12929,7 @@
         <v>0.70155685702998627</v>
       </c>
       <c r="G259" t="s">
-        <v>838</v>
+        <v>845</v>
       </c>
       <c r="H259">
         <v>0.38</v>
@@ -12893,7 +12938,7 @@
         <v>0.89639999999999997</v>
       </c>
       <c r="J259" t="s">
-        <v>839</v>
+        <v>846</v>
       </c>
       <c r="K259">
         <v>0</v>
@@ -12901,13 +12946,13 @@
     </row>
     <row r="260" spans="1:11">
       <c r="A260" t="s">
-        <v>840</v>
+        <v>847</v>
       </c>
       <c r="B260" t="s">
-        <v>841</v>
+        <v>848</v>
       </c>
       <c r="C260" t="s">
-        <v>842</v>
+        <v>849</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -12919,7 +12964,7 @@
         <v>0.6247741645144721</v>
       </c>
       <c r="G260" t="s">
-        <v>843</v>
+        <v>850</v>
       </c>
       <c r="H260">
         <v>0.63</v>
@@ -12936,13 +12981,13 @@
     </row>
     <row r="261" spans="1:11">
       <c r="A261" t="s">
-        <v>844</v>
+        <v>851</v>
       </c>
       <c r="B261" t="s">
-        <v>845</v>
+        <v>852</v>
       </c>
       <c r="C261" t="s">
-        <v>846</v>
+        <v>853</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -12954,7 +12999,7 @@
         <v>0.61378041019317575</v>
       </c>
       <c r="G261" t="s">
-        <v>847</v>
+        <v>854</v>
       </c>
       <c r="H261">
         <v>0.47</v>
@@ -12963,7 +13008,7 @@
         <v>0.84250000000000003</v>
       </c>
       <c r="J261" t="s">
-        <v>848</v>
+        <v>855</v>
       </c>
       <c r="K261">
         <v>0</v>
@@ -12971,13 +13016,13 @@
     </row>
     <row r="262" spans="1:11">
       <c r="A262" t="s">
-        <v>849</v>
+        <v>856</v>
       </c>
       <c r="B262" t="s">
-        <v>850</v>
+        <v>857</v>
       </c>
       <c r="C262" t="s">
-        <v>851</v>
+        <v>858</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -12989,7 +13034,7 @@
         <v>0.68835513277843841</v>
       </c>
       <c r="G262" t="s">
-        <v>852</v>
+        <v>859</v>
       </c>
       <c r="H262">
         <v>0.26</v>
@@ -12998,7 +13043,7 @@
         <v>0.80209999999999992</v>
       </c>
       <c r="J262" t="s">
-        <v>853</v>
+        <v>860</v>
       </c>
       <c r="K262">
         <v>0</v>
@@ -13006,13 +13051,13 @@
     </row>
     <row r="263" spans="1:11">
       <c r="A263" t="s">
-        <v>854</v>
+        <v>861</v>
       </c>
       <c r="B263" t="s">
-        <v>855</v>
+        <v>862</v>
       </c>
       <c r="C263" t="s">
-        <v>856</v>
+        <v>863</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -13024,7 +13069,7 @@
         <v>0.93440094834565979</v>
       </c>
       <c r="G263" t="s">
-        <v>857</v>
+        <v>864</v>
       </c>
       <c r="H263">
         <v>0</v>
@@ -13033,7 +13078,7 @@
         <v>0.90010000000000001</v>
       </c>
       <c r="J263" t="s">
-        <v>858</v>
+        <v>865</v>
       </c>
       <c r="K263">
         <v>0</v>
@@ -13041,13 +13086,13 @@
     </row>
     <row r="264" spans="1:11">
       <c r="A264" t="s">
-        <v>859</v>
+        <v>866</v>
       </c>
       <c r="B264" t="s">
-        <v>860</v>
+        <v>867</v>
       </c>
       <c r="C264" t="s">
-        <v>861</v>
+        <v>868</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -13059,7 +13104,7 @@
         <v>0.52763364298887605</v>
       </c>
       <c r="G264" t="s">
-        <v>862</v>
+        <v>869</v>
       </c>
       <c r="H264">
         <v>0</v>
@@ -13068,7 +13113,7 @@
         <v>0.87620000000000009</v>
       </c>
       <c r="J264" t="s">
-        <v>863</v>
+        <v>870</v>
       </c>
       <c r="K264">
         <v>0</v>
@@ -13076,13 +13121,13 @@
     </row>
     <row r="265" spans="1:11">
       <c r="A265" t="s">
-        <v>864</v>
+        <v>871</v>
       </c>
       <c r="B265" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="C265" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -13094,7 +13139,7 @@
         <v>0.50355774493705519</v>
       </c>
       <c r="G265" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
       <c r="H265">
         <v>0</v>
@@ -13103,7 +13148,7 @@
         <v>0.67669999999999997</v>
       </c>
       <c r="J265" t="s">
-        <v>868</v>
+        <v>875</v>
       </c>
       <c r="K265">
         <v>0</v>
@@ -13111,13 +13156,13 @@
     </row>
     <row r="266" spans="1:11">
       <c r="A266" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B266" t="s">
-        <v>870</v>
+        <v>877</v>
       </c>
       <c r="C266" t="s">
-        <v>871</v>
+        <v>878</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -13129,7 +13174,7 @@
         <v>0.52121822842574161</v>
       </c>
       <c r="G266" t="s">
-        <v>872</v>
+        <v>879</v>
       </c>
       <c r="H266">
         <v>0.17</v>
@@ -13138,7 +13183,7 @@
         <v>0.89410000000000001</v>
       </c>
       <c r="J266" t="s">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="K266">
         <v>0</v>
@@ -13146,13 +13191,13 @@
     </row>
     <row r="267" spans="1:11">
       <c r="A267" t="s">
-        <v>874</v>
+        <v>881</v>
       </c>
       <c r="B267" t="s">
-        <v>875</v>
+        <v>882</v>
       </c>
       <c r="C267" t="s">
-        <v>876</v>
+        <v>883</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -13164,7 +13209,7 @@
         <v>0.24464916656274679</v>
       </c>
       <c r="G267" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="H267">
         <v>0.14000000000000001</v>
@@ -13173,7 +13218,7 @@
         <v>0.96260000000000001</v>
       </c>
       <c r="J267" t="s">
-        <v>878</v>
+        <v>885</v>
       </c>
       <c r="K267">
         <v>0</v>
@@ -13181,13 +13226,13 @@
     </row>
     <row r="268" spans="1:11">
       <c r="A268" t="s">
-        <v>879</v>
+        <v>886</v>
       </c>
       <c r="B268" t="s">
-        <v>880</v>
+        <v>887</v>
       </c>
       <c r="C268" t="s">
-        <v>881</v>
+        <v>888</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -13199,7 +13244,7 @@
         <v>0.42987585923874011</v>
       </c>
       <c r="G268" t="s">
-        <v>882</v>
+        <v>889</v>
       </c>
       <c r="H268">
         <v>0</v>
@@ -13208,7 +13253,7 @@
         <v>0.9335</v>
       </c>
       <c r="J268" t="s">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="K268">
         <v>0</v>
@@ -13216,13 +13261,13 @@
     </row>
     <row r="269" spans="1:11">
       <c r="A269" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="B269" t="s">
-        <v>885</v>
+        <v>892</v>
       </c>
       <c r="C269" t="s">
-        <v>886</v>
+        <v>893</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -13234,7 +13279,7 @@
         <v>0.86196594368483526</v>
       </c>
       <c r="G269" t="s">
-        <v>887</v>
+        <v>894</v>
       </c>
       <c r="H269">
         <v>0.76</v>
@@ -13243,7 +13288,7 @@
         <v>0.94590000000000007</v>
       </c>
       <c r="J269" t="s">
-        <v>888</v>
+        <v>895</v>
       </c>
       <c r="K269">
         <v>0</v>
@@ -13251,13 +13296,13 @@
     </row>
     <row r="270" spans="1:11">
       <c r="A270" t="s">
-        <v>889</v>
+        <v>896</v>
       </c>
       <c r="B270" t="s">
-        <v>890</v>
+        <v>897</v>
       </c>
       <c r="C270" t="s">
-        <v>891</v>
+        <v>898</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -13269,7 +13314,7 @@
         <v>0.88802454698719147</v>
       </c>
       <c r="G270" t="s">
-        <v>892</v>
+        <v>899</v>
       </c>
       <c r="H270">
         <v>0.73</v>
@@ -13278,7 +13323,7 @@
         <v>0.97549999999999992</v>
       </c>
       <c r="J270" t="s">
-        <v>893</v>
+        <v>900</v>
       </c>
       <c r="K270">
         <v>0</v>
@@ -13286,13 +13331,13 @@
     </row>
     <row r="271" spans="1:11">
       <c r="A271" t="s">
-        <v>894</v>
+        <v>901</v>
       </c>
       <c r="B271" t="s">
-        <v>895</v>
+        <v>902</v>
       </c>
       <c r="C271" t="s">
-        <v>896</v>
+        <v>903</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -13304,7 +13349,7 @@
         <v>0.58879799469651517</v>
       </c>
       <c r="G271" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="H271">
         <v>0.16</v>
@@ -13313,7 +13358,7 @@
         <v>0.85709999999999997</v>
       </c>
       <c r="J271" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="K271">
         <v>0</v>
@@ -13321,13 +13366,13 @@
     </row>
     <row r="272" spans="1:11">
       <c r="A272" t="s">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="B272" t="s">
-        <v>900</v>
+        <v>907</v>
       </c>
       <c r="C272" t="s">
-        <v>901</v>
+        <v>908</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -13339,7 +13384,7 @@
         <v>0.66424709652589042</v>
       </c>
       <c r="G272" t="s">
-        <v>902</v>
+        <v>909</v>
       </c>
       <c r="H272">
         <v>0</v>
@@ -13348,7 +13393,7 @@
         <v>0.77150000000000007</v>
       </c>
       <c r="J272" t="s">
-        <v>903</v>
+        <v>910</v>
       </c>
       <c r="K272">
         <v>0</v>
@@ -13356,13 +13401,13 @@
     </row>
     <row r="273" spans="1:11">
       <c r="A273" t="s">
-        <v>904</v>
+        <v>911</v>
       </c>
       <c r="B273" t="s">
-        <v>905</v>
+        <v>912</v>
       </c>
       <c r="C273" t="s">
-        <v>906</v>
+        <v>913</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -13374,7 +13419,7 @@
         <v>0.52442395360121852</v>
       </c>
       <c r="G273" t="s">
-        <v>907</v>
+        <v>914</v>
       </c>
       <c r="H273">
         <v>0</v>
@@ -13383,7 +13428,7 @@
         <v>0.73470000000000002</v>
       </c>
       <c r="J273" t="s">
-        <v>908</v>
+        <v>915</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -13391,13 +13436,13 @@
     </row>
     <row r="274" spans="1:11">
       <c r="A274" t="s">
-        <v>909</v>
+        <v>916</v>
       </c>
       <c r="B274" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
       <c r="C274" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -13409,7 +13454,7 @@
         <v>0.17054273168875969</v>
       </c>
       <c r="G274" t="s">
-        <v>911</v>
+        <v>918</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -13418,7 +13463,7 @@
         <v>0.67669999999999997</v>
       </c>
       <c r="J274" t="s">
-        <v>912</v>
+        <v>919</v>
       </c>
       <c r="K274">
         <v>0</v>
@@ -13426,13 +13471,13 @@
     </row>
     <row r="275" spans="1:11">
       <c r="A275" t="s">
-        <v>913</v>
+        <v>920</v>
       </c>
       <c r="B275" t="s">
-        <v>914</v>
+        <v>921</v>
       </c>
       <c r="C275" t="s">
-        <v>915</v>
+        <v>922</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -13444,7 +13489,7 @@
         <v>0.25958012686025911</v>
       </c>
       <c r="G275" t="s">
-        <v>916</v>
+        <v>923</v>
       </c>
       <c r="H275">
         <v>0</v>
@@ -13453,7 +13498,7 @@
         <v>0.79760000000000009</v>
       </c>
       <c r="J275" t="s">
-        <v>917</v>
+        <v>924</v>
       </c>
       <c r="K275">
         <v>0</v>
@@ -13461,13 +13506,13 @@
     </row>
     <row r="276" spans="1:11">
       <c r="A276" t="s">
-        <v>918</v>
+        <v>925</v>
       </c>
       <c r="B276" t="s">
-        <v>919</v>
+        <v>926</v>
       </c>
       <c r="C276" t="s">
-        <v>920</v>
+        <v>927</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -13479,7 +13524,7 @@
         <v>0.48741343083544247</v>
       </c>
       <c r="G276" t="s">
-        <v>921</v>
+        <v>928</v>
       </c>
       <c r="H276">
         <v>0.52</v>
@@ -13488,7 +13533,7 @@
         <v>0.80959999999999999</v>
       </c>
       <c r="J276" t="s">
-        <v>922</v>
+        <v>929</v>
       </c>
       <c r="K276">
         <v>0</v>
@@ -13496,13 +13541,13 @@
     </row>
     <row r="277" spans="1:11">
       <c r="A277" t="s">
-        <v>923</v>
+        <v>930</v>
       </c>
       <c r="B277" t="s">
-        <v>924</v>
+        <v>931</v>
       </c>
       <c r="C277" t="s">
-        <v>925</v>
+        <v>932</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -13514,7 +13559,7 @@
         <v>0.89602265394280345</v>
       </c>
       <c r="G277" t="s">
-        <v>926</v>
+        <v>933</v>
       </c>
       <c r="H277">
         <v>0.77</v>
@@ -13531,13 +13576,13 @@
     </row>
     <row r="278" spans="1:11">
       <c r="A278" t="s">
-        <v>927</v>
+        <v>934</v>
       </c>
       <c r="B278" t="s">
-        <v>928</v>
+        <v>935</v>
       </c>
       <c r="C278" t="s">
-        <v>928</v>
+        <v>935</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -13566,13 +13611,13 @@
     </row>
     <row r="279" spans="1:11">
       <c r="A279" t="s">
-        <v>929</v>
+        <v>936</v>
       </c>
       <c r="B279" t="s">
-        <v>930</v>
+        <v>937</v>
       </c>
       <c r="C279" t="s">
-        <v>931</v>
+        <v>938</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -13584,7 +13629,7 @@
         <v>0.99997459736828731</v>
       </c>
       <c r="G279" t="s">
-        <v>932</v>
+        <v>939</v>
       </c>
       <c r="H279">
         <v>1</v>
@@ -13593,7 +13638,7 @@
         <v>1</v>
       </c>
       <c r="J279" t="s">
-        <v>933</v>
+        <v>940</v>
       </c>
       <c r="K279">
         <v>0</v>
@@ -13601,13 +13646,13 @@
     </row>
     <row r="280" spans="1:11">
       <c r="A280" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="B280" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="C280" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="D280">
         <v>1</v>
@@ -13636,13 +13681,13 @@
     </row>
     <row r="281" spans="1:11">
       <c r="A281" t="s">
-        <v>936</v>
+        <v>943</v>
       </c>
       <c r="B281" t="s">
-        <v>937</v>
+        <v>944</v>
       </c>
       <c r="C281" t="s">
-        <v>937</v>
+        <v>944</v>
       </c>
       <c r="D281">
         <v>1</v>
@@ -13671,13 +13716,13 @@
     </row>
     <row r="282" spans="1:11">
       <c r="A282" t="s">
-        <v>938</v>
+        <v>945</v>
       </c>
       <c r="B282" t="s">
-        <v>939</v>
+        <v>946</v>
       </c>
       <c r="C282" t="s">
-        <v>939</v>
+        <v>946</v>
       </c>
       <c r="D282">
         <v>1</v>
@@ -13706,13 +13751,13 @@
     </row>
     <row r="283" spans="1:11">
       <c r="A283" t="s">
-        <v>940</v>
+        <v>947</v>
       </c>
       <c r="B283" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
       <c r="C283" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -13724,7 +13769,7 @@
         <v>0.16107144603648099</v>
       </c>
       <c r="G283" t="s">
-        <v>943</v>
+        <v>950</v>
       </c>
       <c r="H283">
         <v>0.15</v>
@@ -13733,7 +13778,7 @@
         <v>8.2400000000000001E-2</v>
       </c>
       <c r="J283" t="s">
-        <v>944</v>
+        <v>951</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -13741,13 +13786,13 @@
     </row>
     <row r="284" spans="1:11">
       <c r="A284" t="s">
-        <v>945</v>
+        <v>952</v>
       </c>
       <c r="B284" t="s">
-        <v>946</v>
+        <v>953</v>
       </c>
       <c r="C284" t="s">
-        <v>947</v>
+        <v>954</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -13759,7 +13804,7 @@
         <v>0.99985185185185188</v>
       </c>
       <c r="G284" t="s">
-        <v>948</v>
+        <v>955</v>
       </c>
       <c r="H284">
         <v>0.92</v>
@@ -13768,7 +13813,7 @@
         <v>0.98939999999999995</v>
       </c>
       <c r="J284" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="K284">
         <v>0</v>
@@ -13776,13 +13821,13 @@
     </row>
     <row r="285" spans="1:11">
       <c r="A285" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
       <c r="B285" t="s">
-        <v>950</v>
+        <v>957</v>
       </c>
       <c r="C285" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -13794,7 +13839,7 @@
         <v>0.99999088788453128</v>
       </c>
       <c r="G285" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
       <c r="H285">
         <v>1</v>
@@ -13811,13 +13856,13 @@
     </row>
     <row r="286" spans="1:11">
       <c r="A286" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
       <c r="B286" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="C286" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -13829,7 +13874,7 @@
         <v>0.40546209674036149</v>
       </c>
       <c r="G286" t="s">
-        <v>956</v>
+        <v>963</v>
       </c>
       <c r="H286">
         <v>0.21</v>
@@ -13838,7 +13883,7 @@
         <v>0.58109999999999995</v>
       </c>
       <c r="J286" t="s">
-        <v>957</v>
+        <v>964</v>
       </c>
       <c r="K286">
         <v>0</v>
@@ -13846,13 +13891,13 @@
     </row>
     <row r="287" spans="1:11">
       <c r="A287" t="s">
-        <v>958</v>
+        <v>965</v>
       </c>
       <c r="B287" t="s">
-        <v>959</v>
+        <v>966</v>
       </c>
       <c r="C287" t="s">
-        <v>959</v>
+        <v>966</v>
       </c>
       <c r="D287">
         <v>1</v>
@@ -13881,13 +13926,13 @@
     </row>
     <row r="288" spans="1:11">
       <c r="A288" t="s">
-        <v>960</v>
+        <v>967</v>
       </c>
       <c r="B288" t="s">
-        <v>961</v>
+        <v>968</v>
       </c>
       <c r="C288" t="s">
-        <v>961</v>
+        <v>968</v>
       </c>
       <c r="D288">
         <v>1</v>
@@ -13916,13 +13961,13 @@
     </row>
     <row r="289" spans="1:11">
       <c r="A289" t="s">
-        <v>962</v>
+        <v>969</v>
       </c>
       <c r="B289" t="s">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="C289" t="s">
-        <v>964</v>
+        <v>971</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -13934,7 +13979,7 @@
         <v>0.99999451303155007</v>
       </c>
       <c r="G289" t="s">
-        <v>965</v>
+        <v>972</v>
       </c>
       <c r="H289">
         <v>0.92</v>
@@ -13943,7 +13988,7 @@
         <v>0.98659999999999992</v>
       </c>
       <c r="J289" t="s">
-        <v>966</v>
+        <v>973</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -13951,13 +13996,13 @@
     </row>
     <row r="290" spans="1:11">
       <c r="A290" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
       <c r="B290" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="C290" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="D290">
         <v>1</v>
@@ -13986,13 +14031,13 @@
     </row>
     <row r="291" spans="1:11">
       <c r="A291" t="s">
-        <v>969</v>
+        <v>976</v>
       </c>
       <c r="B291" t="s">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="C291" t="s">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -14021,13 +14066,13 @@
     </row>
     <row r="292" spans="1:11">
       <c r="A292" t="s">
-        <v>971</v>
+        <v>978</v>
       </c>
       <c r="B292" t="s">
-        <v>972</v>
+        <v>979</v>
       </c>
       <c r="C292" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -14039,7 +14084,7 @@
         <v>0.93487490844375576</v>
       </c>
       <c r="G292" t="s">
-        <v>974</v>
+        <v>981</v>
       </c>
       <c r="H292">
         <v>0.9</v>
@@ -14048,7 +14093,7 @@
         <v>0.9909</v>
       </c>
       <c r="J292" t="s">
-        <v>975</v>
+        <v>982</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -14056,13 +14101,13 @@
     </row>
     <row r="293" spans="1:11">
       <c r="A293" t="s">
-        <v>976</v>
+        <v>983</v>
       </c>
       <c r="B293" t="s">
-        <v>977</v>
+        <v>984</v>
       </c>
       <c r="C293" t="s">
-        <v>977</v>
+        <v>984</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -14091,13 +14136,13 @@
     </row>
     <row r="294" spans="1:11">
       <c r="A294" t="s">
-        <v>978</v>
+        <v>985</v>
       </c>
       <c r="B294" t="s">
-        <v>979</v>
+        <v>986</v>
       </c>
       <c r="C294" t="s">
-        <v>980</v>
+        <v>987</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -14109,7 +14154,7 @@
         <v>0.70304985209989224</v>
       </c>
       <c r="G294" t="s">
-        <v>981</v>
+        <v>988</v>
       </c>
       <c r="H294">
         <v>0.66</v>
@@ -14118,7 +14163,7 @@
         <v>0.97909999999999997</v>
       </c>
       <c r="J294" t="s">
-        <v>982</v>
+        <v>989</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -14126,13 +14171,13 @@
     </row>
     <row r="295" spans="1:11">
       <c r="A295" t="s">
-        <v>983</v>
+        <v>990</v>
       </c>
       <c r="B295" t="s">
-        <v>984</v>
+        <v>991</v>
       </c>
       <c r="C295" t="s">
-        <v>985</v>
+        <v>992</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -14144,7 +14189,7 @@
         <v>0.99999902343750002</v>
       </c>
       <c r="G295" t="s">
-        <v>986</v>
+        <v>993</v>
       </c>
       <c r="H295">
         <v>1</v>
@@ -14153,7 +14198,7 @@
         <v>1</v>
       </c>
       <c r="J295" t="s">
-        <v>987</v>
+        <v>994</v>
       </c>
       <c r="K295">
         <v>0</v>
@@ -14161,13 +14206,13 @@
     </row>
     <row r="296" spans="1:11">
       <c r="A296" t="s">
-        <v>988</v>
+        <v>995</v>
       </c>
       <c r="B296" t="s">
-        <v>989</v>
+        <v>996</v>
       </c>
       <c r="C296" t="s">
-        <v>990</v>
+        <v>997</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -14179,7 +14224,7 @@
         <v>0.99999518411142041</v>
       </c>
       <c r="G296" t="s">
-        <v>991</v>
+        <v>998</v>
       </c>
       <c r="H296">
         <v>1</v>
@@ -14188,7 +14233,7 @@
         <v>1</v>
       </c>
       <c r="J296" t="s">
-        <v>992</v>
+        <v>999</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -14196,13 +14241,13 @@
     </row>
     <row r="297" spans="1:11">
       <c r="A297" t="s">
-        <v>993</v>
+        <v>1000</v>
       </c>
       <c r="B297" t="s">
-        <v>994</v>
+        <v>1001</v>
       </c>
       <c r="C297" t="s">
-        <v>994</v>
+        <v>1001</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -14231,13 +14276,13 @@
     </row>
     <row r="298" spans="1:11">
       <c r="A298" t="s">
-        <v>995</v>
+        <v>1002</v>
       </c>
       <c r="B298" t="s">
-        <v>996</v>
+        <v>1003</v>
       </c>
       <c r="C298" t="s">
-        <v>997</v>
+        <v>1004</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -14249,7 +14294,7 @@
         <v>0.96253492767915849</v>
       </c>
       <c r="G298" t="s">
-        <v>998</v>
+        <v>1005</v>
       </c>
       <c r="H298">
         <v>0.83</v>
@@ -14258,7 +14303,7 @@
         <v>0.9484999999999999</v>
       </c>
       <c r="J298" t="s">
-        <v>999</v>
+        <v>1006</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -14266,13 +14311,13 @@
     </row>
     <row r="299" spans="1:11">
       <c r="A299" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
       <c r="B299" t="s">
-        <v>1001</v>
+        <v>1008</v>
       </c>
       <c r="C299" t="s">
-        <v>1001</v>
+        <v>1008</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -14301,13 +14346,13 @@
     </row>
     <row r="300" spans="1:11">
       <c r="A300" t="s">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="B300" t="s">
-        <v>1003</v>
+        <v>1010</v>
       </c>
       <c r="C300" t="s">
-        <v>1004</v>
+        <v>1011</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -14319,7 +14364,7 @@
         <v>0.96831509702158602</v>
       </c>
       <c r="G300" t="s">
-        <v>1005</v>
+        <v>1012</v>
       </c>
       <c r="H300">
         <v>0.69</v>
@@ -14328,7 +14373,7 @@
         <v>0.87959999999999994</v>
       </c>
       <c r="J300" t="s">
-        <v>975</v>
+        <v>982</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -14336,13 +14381,13 @@
     </row>
     <row r="301" spans="1:11">
       <c r="A301" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="B301" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
       <c r="C301" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
       <c r="D301">
         <v>1</v>
@@ -14371,13 +14416,13 @@
     </row>
     <row r="302" spans="1:11">
       <c r="A302" t="s">
-        <v>1008</v>
+        <v>1015</v>
       </c>
       <c r="B302" t="s">
-        <v>1009</v>
+        <v>1016</v>
       </c>
       <c r="C302" t="s">
-        <v>1010</v>
+        <v>1017</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -14389,7 +14434,7 @@
         <v>0.999996</v>
       </c>
       <c r="G302" t="s">
-        <v>1011</v>
+        <v>1018</v>
       </c>
       <c r="H302">
         <v>1</v>
@@ -14398,7 +14443,7 @@
         <v>1</v>
       </c>
       <c r="J302" t="s">
-        <v>1012</v>
+        <v>1019</v>
       </c>
       <c r="K302">
         <v>0</v>
@@ -14406,13 +14451,13 @@
     </row>
     <row r="303" spans="1:11">
       <c r="A303" t="s">
-        <v>1013</v>
+        <v>1020</v>
       </c>
       <c r="B303" t="s">
-        <v>1014</v>
+        <v>1021</v>
       </c>
       <c r="C303" t="s">
-        <v>1015</v>
+        <v>1022</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -14424,7 +14469,7 @@
         <v>0.74476011756102278</v>
       </c>
       <c r="G303" t="s">
-        <v>1016</v>
+        <v>1023</v>
       </c>
       <c r="H303">
         <v>0.56000000000000005</v>
@@ -14433,7 +14478,7 @@
         <v>0.76290000000000002</v>
       </c>
       <c r="J303" t="s">
-        <v>1017</v>
+        <v>1024</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -14441,13 +14486,13 @@
     </row>
     <row r="304" spans="1:11">
       <c r="A304" t="s">
-        <v>1018</v>
+        <v>1025</v>
       </c>
       <c r="B304" t="s">
-        <v>1019</v>
+        <v>1026</v>
       </c>
       <c r="C304" t="s">
-        <v>1020</v>
+        <v>1027</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -14459,7 +14504,7 @@
         <v>0.64379423183166962</v>
       </c>
       <c r="G304" t="s">
-        <v>1021</v>
+        <v>1028</v>
       </c>
       <c r="H304">
         <v>0.56999999999999995</v>
@@ -14468,7 +14513,7 @@
         <v>0.93209999999999993</v>
       </c>
       <c r="J304" t="s">
-        <v>1022</v>
+        <v>1029</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -14476,13 +14521,13 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305" t="s">
-        <v>1023</v>
+        <v>1030</v>
       </c>
       <c r="B305" t="s">
-        <v>1024</v>
+        <v>1031</v>
       </c>
       <c r="C305" t="s">
-        <v>1024</v>
+        <v>1031</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -14511,13 +14556,13 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306" t="s">
-        <v>1025</v>
+        <v>1032</v>
       </c>
       <c r="B306" t="s">
-        <v>1026</v>
+        <v>1033</v>
       </c>
       <c r="C306" t="s">
-        <v>1027</v>
+        <v>1034</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -14529,7 +14574,7 @@
         <v>0.97417177571210234</v>
       </c>
       <c r="G306" t="s">
-        <v>1028</v>
+        <v>1035</v>
       </c>
       <c r="H306">
         <v>0.93</v>
@@ -14538,7 +14583,7 @@
         <v>0.98209999999999997</v>
       </c>
       <c r="J306" t="s">
-        <v>1029</v>
+        <v>1036</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -14546,13 +14591,13 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307" t="s">
-        <v>1030</v>
+        <v>1037</v>
       </c>
       <c r="B307" t="s">
-        <v>1031</v>
+        <v>1038</v>
       </c>
       <c r="C307" t="s">
-        <v>1031</v>
+        <v>1038</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -14581,13 +14626,13 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308" t="s">
-        <v>1032</v>
+        <v>1039</v>
       </c>
       <c r="B308" t="s">
-        <v>1033</v>
+        <v>1040</v>
       </c>
       <c r="C308" t="s">
-        <v>1034</v>
+        <v>1041</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -14599,7 +14644,7 @@
         <v>0.98664022774046589</v>
       </c>
       <c r="G308" t="s">
-        <v>1035</v>
+        <v>1042</v>
       </c>
       <c r="H308">
         <v>0.97</v>
@@ -14608,7 +14653,7 @@
         <v>0.98909999999999998</v>
       </c>
       <c r="J308" t="s">
-        <v>1036</v>
+        <v>1043</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -14616,13 +14661,13 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309" t="s">
-        <v>1037</v>
+        <v>1044</v>
       </c>
       <c r="B309" t="s">
-        <v>1038</v>
+        <v>1045</v>
       </c>
       <c r="C309" t="s">
-        <v>1039</v>
+        <v>1046</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -14634,7 +14679,7 @@
         <v>0.99995890523547304</v>
       </c>
       <c r="G309" t="s">
-        <v>1040</v>
+        <v>1047</v>
       </c>
       <c r="H309">
         <v>1</v>
@@ -14643,7 +14688,7 @@
         <v>1</v>
       </c>
       <c r="J309" t="s">
-        <v>933</v>
+        <v>940</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -14651,13 +14696,13 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310" t="s">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="B310" t="s">
-        <v>1042</v>
+        <v>1049</v>
       </c>
       <c r="C310" t="s">
-        <v>1042</v>
+        <v>1049</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -14686,13 +14731,13 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311" t="s">
-        <v>1043</v>
+        <v>1050</v>
       </c>
       <c r="B311" t="s">
-        <v>1044</v>
+        <v>1051</v>
       </c>
       <c r="C311" t="s">
-        <v>1045</v>
+        <v>1052</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -14704,7 +14749,7 @@
         <v>0.99998928326474623</v>
       </c>
       <c r="G311" t="s">
-        <v>1046</v>
+        <v>1053</v>
       </c>
       <c r="H311">
         <v>1</v>
@@ -14721,13 +14766,13 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312" t="s">
-        <v>1047</v>
+        <v>1054</v>
       </c>
       <c r="B312" t="s">
-        <v>1048</v>
+        <v>1055</v>
       </c>
       <c r="C312" t="s">
-        <v>1049</v>
+        <v>1056</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -14739,7 +14784,7 @@
         <v>0.97341886358453711</v>
       </c>
       <c r="G312" t="s">
-        <v>1050</v>
+        <v>1057</v>
       </c>
       <c r="H312">
         <v>0.94</v>
@@ -14748,7 +14793,7 @@
         <v>0.97719999999999996</v>
       </c>
       <c r="J312" t="s">
-        <v>1051</v>
+        <v>1058</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -14756,13 +14801,13 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313" t="s">
-        <v>1052</v>
+        <v>1059</v>
       </c>
       <c r="B313" t="s">
-        <v>1053</v>
+        <v>1060</v>
       </c>
       <c r="C313" t="s">
-        <v>1054</v>
+        <v>1061</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -14774,7 +14819,7 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313" t="s">
-        <v>1055</v>
+        <v>1062</v>
       </c>
       <c r="H313">
         <v>0.89</v>
@@ -14783,7 +14828,7 @@
         <v>0.9756999999999999</v>
       </c>
       <c r="J313" t="s">
-        <v>1056</v>
+        <v>1063</v>
       </c>
       <c r="K313">
         <v>0</v>
@@ -14791,13 +14836,13 @@
     </row>
     <row r="314" spans="1:11">
       <c r="A314" t="s">
-        <v>1057</v>
+        <v>1064</v>
       </c>
       <c r="B314" t="s">
-        <v>1058</v>
+        <v>1065</v>
       </c>
       <c r="C314" t="s">
-        <v>1059</v>
+        <v>1066</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -14809,7 +14854,7 @@
         <v>0.75858170895276666</v>
       </c>
       <c r="G314" t="s">
-        <v>1060</v>
+        <v>1067</v>
       </c>
       <c r="H314">
         <v>0.54</v>
@@ -14818,7 +14863,7 @@
         <v>0.68030000000000002</v>
       </c>
       <c r="J314" t="s">
-        <v>1061</v>
+        <v>1068</v>
       </c>
       <c r="K314">
         <v>0</v>
@@ -14826,13 +14871,13 @@
     </row>
     <row r="315" spans="1:11">
       <c r="A315" t="s">
-        <v>1062</v>
+        <v>1069</v>
       </c>
       <c r="B315" t="s">
-        <v>1063</v>
+        <v>1070</v>
       </c>
       <c r="C315" t="s">
-        <v>1064</v>
+        <v>1071</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -14844,7 +14889,7 @@
         <v>0.998317618783509</v>
       </c>
       <c r="G315" t="s">
-        <v>1065</v>
+        <v>1072</v>
       </c>
       <c r="H315">
         <v>0.9</v>
@@ -14853,7 +14898,7 @@
         <v>0.97470000000000001</v>
       </c>
       <c r="J315" t="s">
-        <v>1066</v>
+        <v>1073</v>
       </c>
       <c r="K315">
         <v>0</v>
@@ -14861,13 +14906,13 @@
     </row>
     <row r="316" spans="1:11">
       <c r="A316" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="B316" t="s">
-        <v>1068</v>
+        <v>1075</v>
       </c>
       <c r="C316" t="s">
-        <v>1069</v>
+        <v>1076</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -14879,7 +14924,7 @@
         <v>0.95598287878305699</v>
       </c>
       <c r="G316" t="s">
-        <v>1070</v>
+        <v>1077</v>
       </c>
       <c r="H316">
         <v>0.92</v>
@@ -14888,7 +14933,7 @@
         <v>0.97089999999999999</v>
       </c>
       <c r="J316" t="s">
-        <v>1071</v>
+        <v>1078</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -14896,13 +14941,13 @@
     </row>
     <row r="317" spans="1:11">
       <c r="A317" t="s">
-        <v>1072</v>
+        <v>1079</v>
       </c>
       <c r="B317" t="s">
-        <v>1073</v>
+        <v>1080</v>
       </c>
       <c r="C317" t="s">
-        <v>1073</v>
+        <v>1080</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -14931,13 +14976,13 @@
     </row>
     <row r="318" spans="1:11">
       <c r="A318" t="s">
-        <v>1074</v>
+        <v>1081</v>
       </c>
       <c r="B318" t="s">
-        <v>1075</v>
+        <v>1082</v>
       </c>
       <c r="C318" t="s">
-        <v>1076</v>
+        <v>1083</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -14949,7 +14994,7 @@
         <v>0.95178740438847254</v>
       </c>
       <c r="G318" t="s">
-        <v>1077</v>
+        <v>1084</v>
       </c>
       <c r="H318">
         <v>0.9</v>
@@ -14958,7 +15003,7 @@
         <v>0.97430000000000005</v>
       </c>
       <c r="J318" t="s">
-        <v>1078</v>
+        <v>1085</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -14966,13 +15011,13 @@
     </row>
     <row r="319" spans="1:11">
       <c r="A319" t="s">
-        <v>1079</v>
+        <v>1086</v>
       </c>
       <c r="B319" t="s">
-        <v>1080</v>
+        <v>1087</v>
       </c>
       <c r="C319" t="s">
-        <v>1081</v>
+        <v>1088</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -14984,7 +15029,7 @@
         <v>0.70336391437308876</v>
       </c>
       <c r="G319" t="s">
-        <v>1082</v>
+        <v>1089</v>
       </c>
       <c r="H319">
         <v>0.41</v>
@@ -14993,7 +15038,7 @@
         <v>0.80920000000000003</v>
       </c>
       <c r="J319" t="s">
-        <v>1083</v>
+        <v>1090</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -15001,13 +15046,13 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320" t="s">
-        <v>1084</v>
+        <v>1091</v>
       </c>
       <c r="B320" t="s">
-        <v>1085</v>
+        <v>1092</v>
       </c>
       <c r="C320" t="s">
-        <v>1085</v>
+        <v>1092</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -15036,13 +15081,13 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1086</v>
+        <v>1093</v>
       </c>
       <c r="B321" t="s">
-        <v>1087</v>
+        <v>1094</v>
       </c>
       <c r="C321" t="s">
-        <v>1088</v>
+        <v>1095</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -15054,7 +15099,7 @@
         <v>0.99849640734645617</v>
       </c>
       <c r="G321" t="s">
-        <v>1089</v>
+        <v>1096</v>
       </c>
       <c r="H321">
         <v>0.98</v>
@@ -15063,7 +15108,7 @@
         <v>0.99470000000000003</v>
       </c>
       <c r="J321" t="s">
-        <v>1090</v>
+        <v>1097</v>
       </c>
       <c r="K321">
         <v>0</v>
@@ -15071,13 +15116,13 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1091</v>
+        <v>1098</v>
       </c>
       <c r="B322" t="s">
-        <v>1092</v>
+        <v>1099</v>
       </c>
       <c r="C322" t="s">
-        <v>1092</v>
+        <v>1099</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -15106,13 +15151,13 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1093</v>
+        <v>1100</v>
       </c>
       <c r="B323" t="s">
-        <v>1094</v>
+        <v>1101</v>
       </c>
       <c r="C323" t="s">
-        <v>1094</v>
+        <v>1101</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -15141,13 +15186,13 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1095</v>
+        <v>1102</v>
       </c>
       <c r="B324" t="s">
-        <v>1096</v>
+        <v>1103</v>
       </c>
       <c r="C324" t="s">
-        <v>1097</v>
+        <v>1104</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -15159,7 +15204,7 @@
         <v>0.99690437876548454</v>
       </c>
       <c r="G324" t="s">
-        <v>1098</v>
+        <v>1105</v>
       </c>
       <c r="H324">
         <v>0.95</v>
@@ -15168,7 +15213,7 @@
         <v>0.98730000000000007</v>
       </c>
       <c r="J324" t="s">
-        <v>1099</v>
+        <v>1106</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -15176,13 +15221,13 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1100</v>
+        <v>1107</v>
       </c>
       <c r="B325" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
       <c r="C325" t="s">
-        <v>1102</v>
+        <v>1109</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -15194,7 +15239,7 @@
         <v>0.9999968246710359</v>
       </c>
       <c r="G325" t="s">
-        <v>1103</v>
+        <v>1110</v>
       </c>
       <c r="H325">
         <v>1</v>
@@ -15203,7 +15248,7 @@
         <v>1</v>
       </c>
       <c r="J325" t="s">
-        <v>1104</v>
+        <v>1111</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -15211,13 +15256,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1105</v>
+        <v>1112</v>
       </c>
       <c r="B326" t="s">
-        <v>1106</v>
+        <v>1113</v>
       </c>
       <c r="C326" t="s">
-        <v>1106</v>
+        <v>1113</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -15246,13 +15291,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1107</v>
+        <v>1114</v>
       </c>
       <c r="B327" t="s">
-        <v>1108</v>
+        <v>1115</v>
       </c>
       <c r="C327" t="s">
-        <v>1108</v>
+        <v>1115</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Aggiunte nuove analisi su CodeT5_770
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/Analisi_CodeT5_770.xlsx
+++ b/HE/W_in_progress/Analisi_CodeT5_770.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81B46834-1967-40AD-AD3A-13FAE31FCD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F32A0078-DD93-4352-B664-98BE0AB71245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1123">
   <si>
     <t>IN</t>
   </si>
@@ -2382,6 +2382,9 @@
     <t>0.4770642152781753</t>
   </si>
   <si>
+    <t>Non genera numeri pseudo casuali</t>
+  </si>
+  <si>
     <t>Create a configurable clock divider</t>
   </si>
   <si>
@@ -2394,6 +2397,9 @@
     <t>0.4971751412429379</t>
   </si>
   <si>
+    <t>Non è un divisore di frequnza</t>
+  </si>
+  <si>
     <t>Write an astable multivibrator with the signals clk and reset as input and the signal oscillating_out as output.</t>
   </si>
   <si>
@@ -2409,6 +2415,9 @@
     <t>0.708333328342014</t>
   </si>
   <si>
+    <t>E' un astable multivibrator</t>
+  </si>
+  <si>
     <t>Define a rotating priority encoder with the signal request (N-bit) as input and the signals grant (log2N-bit), valid, and rotation_bit as output.</t>
   </si>
   <si>
@@ -2424,6 +2433,9 @@
     <t>0.8730158680209121</t>
   </si>
   <si>
+    <t>Logica errata</t>
+  </si>
+  <si>
     <t>Generate a floating-point adder of N-bit with the signals A (N-bit) and B (N-bit) as input and the signal sum (N-bit) as output.</t>
   </si>
   <si>
@@ -2454,6 +2466,9 @@
     <t>0.6511627857409411</t>
   </si>
   <si>
+    <t>Non è il comparatore richiesto</t>
+  </si>
+  <si>
     <t>Define a 2-to-1 multiplexer with the signals data0, data1, and select as input and the signal data_out as output.</t>
   </si>
   <si>
@@ -2484,6 +2499,9 @@
     <t>0.49999999555555563</t>
   </si>
   <si>
+    <t>Non è un SPI master</t>
+  </si>
+  <si>
     <t>Detect falling edge of a signal using a process.</t>
   </si>
   <si>
@@ -2497,6 +2515,9 @@
   </si>
   <si>
     <t>0.42105262659279785</t>
+  </si>
+  <si>
+    <t>Detecta i falling edge</t>
   </si>
   <si>
     <t>Define a universal shift register of P-bit with the signals clock, shift_enable, shift_direction, and serial_in as input and the signals parallel_out (P-bit) and serial_out as output.</t>
@@ -3751,8 +3772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="C249" sqref="C249"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="K256" sqref="K256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12488,16 +12509,19 @@
       <c r="K246">
         <v>0</v>
       </c>
+      <c r="L246" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="247" spans="1:12">
       <c r="A247" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B247" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C247" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -12509,7 +12533,7 @@
         <v>0.51524183187482964</v>
       </c>
       <c r="G247" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="H247">
         <v>0.24</v>
@@ -12523,16 +12547,19 @@
       <c r="K247">
         <v>0</v>
       </c>
+      <c r="L247" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="248" spans="1:12">
       <c r="A248" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="B248" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="C248" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -12544,7 +12571,7 @@
         <v>0.78286006472129221</v>
       </c>
       <c r="G248" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="H248">
         <v>0.31</v>
@@ -12553,21 +12580,24 @@
         <v>0.875</v>
       </c>
       <c r="J248" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="K248">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L248" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="249" spans="1:12">
       <c r="A249" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="B249" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="C249" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -12579,7 +12609,7 @@
         <v>0.70670746171322651</v>
       </c>
       <c r="G249" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="H249">
         <v>0.56999999999999995</v>
@@ -12588,21 +12618,24 @@
         <v>0.83079999999999998</v>
       </c>
       <c r="J249" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="K249">
         <v>0</v>
+      </c>
+      <c r="L249" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="250" spans="1:12">
       <c r="A250" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="B250" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="C250" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -12614,7 +12647,7 @@
         <v>0.55878820772884119</v>
       </c>
       <c r="G250" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="H250">
         <v>0.38</v>
@@ -12623,21 +12656,21 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="J250" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="K250">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:12">
       <c r="A251" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="B251" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="C251" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -12649,7 +12682,7 @@
         <v>0.50052628839754476</v>
       </c>
       <c r="G251" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="H251">
         <v>0.42</v>
@@ -12658,21 +12691,24 @@
         <v>0.87659999999999993</v>
       </c>
       <c r="J251" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="K251">
         <v>0</v>
+      </c>
+      <c r="L251" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="252" spans="1:12">
       <c r="A252" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
       <c r="B252" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="C252" t="s">
-        <v>809</v>
+        <v>814</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -12684,7 +12720,7 @@
         <v>0.67954376611458289</v>
       </c>
       <c r="G252" t="s">
-        <v>810</v>
+        <v>815</v>
       </c>
       <c r="H252">
         <v>0.5</v>
@@ -12693,21 +12729,21 @@
         <v>0.7722</v>
       </c>
       <c r="J252" t="s">
-        <v>811</v>
+        <v>816</v>
       </c>
       <c r="K252">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="1:12">
       <c r="A253" t="s">
-        <v>812</v>
+        <v>817</v>
       </c>
       <c r="B253" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="C253" t="s">
-        <v>814</v>
+        <v>819</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -12719,7 +12755,7 @@
         <v>0.26743188647338118</v>
       </c>
       <c r="G253" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="H253">
         <v>0</v>
@@ -12728,21 +12764,24 @@
         <v>0.84050000000000002</v>
       </c>
       <c r="J253" t="s">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="K253">
         <v>0</v>
+      </c>
+      <c r="L253" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="254" spans="1:12">
       <c r="A254" t="s">
-        <v>817</v>
+        <v>823</v>
       </c>
       <c r="B254" t="s">
-        <v>818</v>
+        <v>824</v>
       </c>
       <c r="C254" t="s">
-        <v>819</v>
+        <v>825</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -12754,7 +12793,7 @@
         <v>0.61614612178272654</v>
       </c>
       <c r="G254" t="s">
-        <v>820</v>
+        <v>826</v>
       </c>
       <c r="H254">
         <v>0</v>
@@ -12763,21 +12802,24 @@
         <v>0.82230000000000003</v>
       </c>
       <c r="J254" t="s">
-        <v>821</v>
+        <v>827</v>
       </c>
       <c r="K254">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L254" t="s">
+        <v>828</v>
       </c>
     </row>
     <row r="255" spans="1:12">
       <c r="A255" t="s">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c r="B255" t="s">
-        <v>823</v>
+        <v>830</v>
       </c>
       <c r="C255" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -12789,7 +12831,7 @@
         <v>0.81386184861469513</v>
       </c>
       <c r="G255" t="s">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c r="H255">
         <v>0.67</v>
@@ -12798,21 +12840,21 @@
         <v>0.87769999999999992</v>
       </c>
       <c r="J255" t="s">
-        <v>826</v>
+        <v>833</v>
       </c>
       <c r="K255">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256" spans="1:12">
       <c r="A256" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="B256" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="C256" t="s">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -12824,7 +12866,7 @@
         <v>0.34146754595961881</v>
       </c>
       <c r="G256" t="s">
-        <v>830</v>
+        <v>837</v>
       </c>
       <c r="H256">
         <v>0.05</v>
@@ -12833,7 +12875,7 @@
         <v>0.89029999999999998</v>
       </c>
       <c r="J256" t="s">
-        <v>831</v>
+        <v>838</v>
       </c>
       <c r="K256">
         <v>0</v>
@@ -12841,13 +12883,13 @@
     </row>
     <row r="257" spans="1:11">
       <c r="A257" t="s">
-        <v>832</v>
+        <v>839</v>
       </c>
       <c r="B257" t="s">
-        <v>833</v>
+        <v>840</v>
       </c>
       <c r="C257" t="s">
-        <v>834</v>
+        <v>841</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -12859,7 +12901,7 @@
         <v>0.52996093454314475</v>
       </c>
       <c r="G257" t="s">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="H257">
         <v>0</v>
@@ -12868,7 +12910,7 @@
         <v>0.86849999999999994</v>
       </c>
       <c r="J257" t="s">
-        <v>836</v>
+        <v>843</v>
       </c>
       <c r="K257">
         <v>0</v>
@@ -12876,13 +12918,13 @@
     </row>
     <row r="258" spans="1:11">
       <c r="A258" t="s">
-        <v>837</v>
+        <v>844</v>
       </c>
       <c r="B258" t="s">
-        <v>838</v>
+        <v>845</v>
       </c>
       <c r="C258" t="s">
-        <v>839</v>
+        <v>846</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -12894,7 +12936,7 @@
         <v>0.33777001839693588</v>
       </c>
       <c r="G258" t="s">
-        <v>840</v>
+        <v>847</v>
       </c>
       <c r="H258">
         <v>0.11</v>
@@ -12903,7 +12945,7 @@
         <v>0.87250000000000005</v>
       </c>
       <c r="J258" t="s">
-        <v>841</v>
+        <v>848</v>
       </c>
       <c r="K258">
         <v>0</v>
@@ -12911,13 +12953,13 @@
     </row>
     <row r="259" spans="1:11">
       <c r="A259" t="s">
-        <v>842</v>
+        <v>849</v>
       </c>
       <c r="B259" t="s">
-        <v>843</v>
+        <v>850</v>
       </c>
       <c r="C259" t="s">
-        <v>844</v>
+        <v>851</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -12929,7 +12971,7 @@
         <v>0.70155685702998627</v>
       </c>
       <c r="G259" t="s">
-        <v>845</v>
+        <v>852</v>
       </c>
       <c r="H259">
         <v>0.38</v>
@@ -12938,7 +12980,7 @@
         <v>0.89639999999999997</v>
       </c>
       <c r="J259" t="s">
-        <v>846</v>
+        <v>853</v>
       </c>
       <c r="K259">
         <v>0</v>
@@ -12946,13 +12988,13 @@
     </row>
     <row r="260" spans="1:11">
       <c r="A260" t="s">
-        <v>847</v>
+        <v>854</v>
       </c>
       <c r="B260" t="s">
-        <v>848</v>
+        <v>855</v>
       </c>
       <c r="C260" t="s">
-        <v>849</v>
+        <v>856</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -12964,7 +13006,7 @@
         <v>0.6247741645144721</v>
       </c>
       <c r="G260" t="s">
-        <v>850</v>
+        <v>857</v>
       </c>
       <c r="H260">
         <v>0.63</v>
@@ -12981,13 +13023,13 @@
     </row>
     <row r="261" spans="1:11">
       <c r="A261" t="s">
-        <v>851</v>
+        <v>858</v>
       </c>
       <c r="B261" t="s">
-        <v>852</v>
+        <v>859</v>
       </c>
       <c r="C261" t="s">
-        <v>853</v>
+        <v>860</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -12999,7 +13041,7 @@
         <v>0.61378041019317575</v>
       </c>
       <c r="G261" t="s">
-        <v>854</v>
+        <v>861</v>
       </c>
       <c r="H261">
         <v>0.47</v>
@@ -13008,7 +13050,7 @@
         <v>0.84250000000000003</v>
       </c>
       <c r="J261" t="s">
-        <v>855</v>
+        <v>862</v>
       </c>
       <c r="K261">
         <v>0</v>
@@ -13016,13 +13058,13 @@
     </row>
     <row r="262" spans="1:11">
       <c r="A262" t="s">
-        <v>856</v>
+        <v>863</v>
       </c>
       <c r="B262" t="s">
-        <v>857</v>
+        <v>864</v>
       </c>
       <c r="C262" t="s">
-        <v>858</v>
+        <v>865</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -13034,7 +13076,7 @@
         <v>0.68835513277843841</v>
       </c>
       <c r="G262" t="s">
-        <v>859</v>
+        <v>866</v>
       </c>
       <c r="H262">
         <v>0.26</v>
@@ -13043,7 +13085,7 @@
         <v>0.80209999999999992</v>
       </c>
       <c r="J262" t="s">
-        <v>860</v>
+        <v>867</v>
       </c>
       <c r="K262">
         <v>0</v>
@@ -13051,13 +13093,13 @@
     </row>
     <row r="263" spans="1:11">
       <c r="A263" t="s">
-        <v>861</v>
+        <v>868</v>
       </c>
       <c r="B263" t="s">
-        <v>862</v>
+        <v>869</v>
       </c>
       <c r="C263" t="s">
-        <v>863</v>
+        <v>870</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -13069,7 +13111,7 @@
         <v>0.93440094834565979</v>
       </c>
       <c r="G263" t="s">
-        <v>864</v>
+        <v>871</v>
       </c>
       <c r="H263">
         <v>0</v>
@@ -13078,7 +13120,7 @@
         <v>0.90010000000000001</v>
       </c>
       <c r="J263" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="K263">
         <v>0</v>
@@ -13086,13 +13128,13 @@
     </row>
     <row r="264" spans="1:11">
       <c r="A264" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="B264" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
       <c r="C264" t="s">
-        <v>868</v>
+        <v>875</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -13104,7 +13146,7 @@
         <v>0.52763364298887605</v>
       </c>
       <c r="G264" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="H264">
         <v>0</v>
@@ -13113,7 +13155,7 @@
         <v>0.87620000000000009</v>
       </c>
       <c r="J264" t="s">
-        <v>870</v>
+        <v>877</v>
       </c>
       <c r="K264">
         <v>0</v>
@@ -13121,13 +13163,13 @@
     </row>
     <row r="265" spans="1:11">
       <c r="A265" t="s">
-        <v>871</v>
+        <v>878</v>
       </c>
       <c r="B265" t="s">
-        <v>872</v>
+        <v>879</v>
       </c>
       <c r="C265" t="s">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -13139,7 +13181,7 @@
         <v>0.50355774493705519</v>
       </c>
       <c r="G265" t="s">
-        <v>874</v>
+        <v>881</v>
       </c>
       <c r="H265">
         <v>0</v>
@@ -13148,7 +13190,7 @@
         <v>0.67669999999999997</v>
       </c>
       <c r="J265" t="s">
-        <v>875</v>
+        <v>882</v>
       </c>
       <c r="K265">
         <v>0</v>
@@ -13156,13 +13198,13 @@
     </row>
     <row r="266" spans="1:11">
       <c r="A266" t="s">
-        <v>876</v>
+        <v>883</v>
       </c>
       <c r="B266" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="C266" t="s">
-        <v>878</v>
+        <v>885</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -13174,7 +13216,7 @@
         <v>0.52121822842574161</v>
       </c>
       <c r="G266" t="s">
-        <v>879</v>
+        <v>886</v>
       </c>
       <c r="H266">
         <v>0.17</v>
@@ -13183,7 +13225,7 @@
         <v>0.89410000000000001</v>
       </c>
       <c r="J266" t="s">
-        <v>880</v>
+        <v>887</v>
       </c>
       <c r="K266">
         <v>0</v>
@@ -13191,13 +13233,13 @@
     </row>
     <row r="267" spans="1:11">
       <c r="A267" t="s">
-        <v>881</v>
+        <v>888</v>
       </c>
       <c r="B267" t="s">
-        <v>882</v>
+        <v>889</v>
       </c>
       <c r="C267" t="s">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -13209,7 +13251,7 @@
         <v>0.24464916656274679</v>
       </c>
       <c r="G267" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="H267">
         <v>0.14000000000000001</v>
@@ -13218,7 +13260,7 @@
         <v>0.96260000000000001</v>
       </c>
       <c r="J267" t="s">
-        <v>885</v>
+        <v>892</v>
       </c>
       <c r="K267">
         <v>0</v>
@@ -13226,13 +13268,13 @@
     </row>
     <row r="268" spans="1:11">
       <c r="A268" t="s">
-        <v>886</v>
+        <v>893</v>
       </c>
       <c r="B268" t="s">
-        <v>887</v>
+        <v>894</v>
       </c>
       <c r="C268" t="s">
-        <v>888</v>
+        <v>895</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -13244,7 +13286,7 @@
         <v>0.42987585923874011</v>
       </c>
       <c r="G268" t="s">
-        <v>889</v>
+        <v>896</v>
       </c>
       <c r="H268">
         <v>0</v>
@@ -13253,7 +13295,7 @@
         <v>0.9335</v>
       </c>
       <c r="J268" t="s">
-        <v>890</v>
+        <v>897</v>
       </c>
       <c r="K268">
         <v>0</v>
@@ -13261,13 +13303,13 @@
     </row>
     <row r="269" spans="1:11">
       <c r="A269" t="s">
-        <v>891</v>
+        <v>898</v>
       </c>
       <c r="B269" t="s">
-        <v>892</v>
+        <v>899</v>
       </c>
       <c r="C269" t="s">
-        <v>893</v>
+        <v>900</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -13279,7 +13321,7 @@
         <v>0.86196594368483526</v>
       </c>
       <c r="G269" t="s">
-        <v>894</v>
+        <v>901</v>
       </c>
       <c r="H269">
         <v>0.76</v>
@@ -13288,7 +13330,7 @@
         <v>0.94590000000000007</v>
       </c>
       <c r="J269" t="s">
-        <v>895</v>
+        <v>902</v>
       </c>
       <c r="K269">
         <v>0</v>
@@ -13296,13 +13338,13 @@
     </row>
     <row r="270" spans="1:11">
       <c r="A270" t="s">
-        <v>896</v>
+        <v>903</v>
       </c>
       <c r="B270" t="s">
-        <v>897</v>
+        <v>904</v>
       </c>
       <c r="C270" t="s">
-        <v>898</v>
+        <v>905</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -13314,7 +13356,7 @@
         <v>0.88802454698719147</v>
       </c>
       <c r="G270" t="s">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="H270">
         <v>0.73</v>
@@ -13323,7 +13365,7 @@
         <v>0.97549999999999992</v>
       </c>
       <c r="J270" t="s">
-        <v>900</v>
+        <v>907</v>
       </c>
       <c r="K270">
         <v>0</v>
@@ -13331,13 +13373,13 @@
     </row>
     <row r="271" spans="1:11">
       <c r="A271" t="s">
-        <v>901</v>
+        <v>908</v>
       </c>
       <c r="B271" t="s">
-        <v>902</v>
+        <v>909</v>
       </c>
       <c r="C271" t="s">
-        <v>903</v>
+        <v>910</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -13349,7 +13391,7 @@
         <v>0.58879799469651517</v>
       </c>
       <c r="G271" t="s">
-        <v>904</v>
+        <v>911</v>
       </c>
       <c r="H271">
         <v>0.16</v>
@@ -13358,7 +13400,7 @@
         <v>0.85709999999999997</v>
       </c>
       <c r="J271" t="s">
-        <v>905</v>
+        <v>912</v>
       </c>
       <c r="K271">
         <v>0</v>
@@ -13366,13 +13408,13 @@
     </row>
     <row r="272" spans="1:11">
       <c r="A272" t="s">
-        <v>906</v>
+        <v>913</v>
       </c>
       <c r="B272" t="s">
-        <v>907</v>
+        <v>914</v>
       </c>
       <c r="C272" t="s">
-        <v>908</v>
+        <v>915</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -13384,7 +13426,7 @@
         <v>0.66424709652589042</v>
       </c>
       <c r="G272" t="s">
-        <v>909</v>
+        <v>916</v>
       </c>
       <c r="H272">
         <v>0</v>
@@ -13393,7 +13435,7 @@
         <v>0.77150000000000007</v>
       </c>
       <c r="J272" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
       <c r="K272">
         <v>0</v>
@@ -13401,13 +13443,13 @@
     </row>
     <row r="273" spans="1:11">
       <c r="A273" t="s">
-        <v>911</v>
+        <v>918</v>
       </c>
       <c r="B273" t="s">
-        <v>912</v>
+        <v>919</v>
       </c>
       <c r="C273" t="s">
-        <v>913</v>
+        <v>920</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -13419,7 +13461,7 @@
         <v>0.52442395360121852</v>
       </c>
       <c r="G273" t="s">
-        <v>914</v>
+        <v>921</v>
       </c>
       <c r="H273">
         <v>0</v>
@@ -13428,7 +13470,7 @@
         <v>0.73470000000000002</v>
       </c>
       <c r="J273" t="s">
-        <v>915</v>
+        <v>922</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -13436,13 +13478,13 @@
     </row>
     <row r="274" spans="1:11">
       <c r="A274" t="s">
-        <v>916</v>
+        <v>923</v>
       </c>
       <c r="B274" t="s">
-        <v>917</v>
+        <v>924</v>
       </c>
       <c r="C274" t="s">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -13454,7 +13496,7 @@
         <v>0.17054273168875969</v>
       </c>
       <c r="G274" t="s">
-        <v>918</v>
+        <v>925</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -13463,7 +13505,7 @@
         <v>0.67669999999999997</v>
       </c>
       <c r="J274" t="s">
-        <v>919</v>
+        <v>926</v>
       </c>
       <c r="K274">
         <v>0</v>
@@ -13471,13 +13513,13 @@
     </row>
     <row r="275" spans="1:11">
       <c r="A275" t="s">
-        <v>920</v>
+        <v>927</v>
       </c>
       <c r="B275" t="s">
-        <v>921</v>
+        <v>928</v>
       </c>
       <c r="C275" t="s">
-        <v>922</v>
+        <v>929</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -13489,7 +13531,7 @@
         <v>0.25958012686025911</v>
       </c>
       <c r="G275" t="s">
-        <v>923</v>
+        <v>930</v>
       </c>
       <c r="H275">
         <v>0</v>
@@ -13498,7 +13540,7 @@
         <v>0.79760000000000009</v>
       </c>
       <c r="J275" t="s">
-        <v>924</v>
+        <v>931</v>
       </c>
       <c r="K275">
         <v>0</v>
@@ -13506,13 +13548,13 @@
     </row>
     <row r="276" spans="1:11">
       <c r="A276" t="s">
-        <v>925</v>
+        <v>932</v>
       </c>
       <c r="B276" t="s">
-        <v>926</v>
+        <v>933</v>
       </c>
       <c r="C276" t="s">
-        <v>927</v>
+        <v>934</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -13524,7 +13566,7 @@
         <v>0.48741343083544247</v>
       </c>
       <c r="G276" t="s">
-        <v>928</v>
+        <v>935</v>
       </c>
       <c r="H276">
         <v>0.52</v>
@@ -13533,7 +13575,7 @@
         <v>0.80959999999999999</v>
       </c>
       <c r="J276" t="s">
-        <v>929</v>
+        <v>936</v>
       </c>
       <c r="K276">
         <v>0</v>
@@ -13541,13 +13583,13 @@
     </row>
     <row r="277" spans="1:11">
       <c r="A277" t="s">
-        <v>930</v>
+        <v>937</v>
       </c>
       <c r="B277" t="s">
-        <v>931</v>
+        <v>938</v>
       </c>
       <c r="C277" t="s">
-        <v>932</v>
+        <v>939</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -13559,7 +13601,7 @@
         <v>0.89602265394280345</v>
       </c>
       <c r="G277" t="s">
-        <v>933</v>
+        <v>940</v>
       </c>
       <c r="H277">
         <v>0.77</v>
@@ -13576,13 +13618,13 @@
     </row>
     <row r="278" spans="1:11">
       <c r="A278" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="B278" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="C278" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -13611,13 +13653,13 @@
     </row>
     <row r="279" spans="1:11">
       <c r="A279" t="s">
-        <v>936</v>
+        <v>943</v>
       </c>
       <c r="B279" t="s">
-        <v>937</v>
+        <v>944</v>
       </c>
       <c r="C279" t="s">
-        <v>938</v>
+        <v>945</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -13629,7 +13671,7 @@
         <v>0.99997459736828731</v>
       </c>
       <c r="G279" t="s">
-        <v>939</v>
+        <v>946</v>
       </c>
       <c r="H279">
         <v>1</v>
@@ -13638,7 +13680,7 @@
         <v>1</v>
       </c>
       <c r="J279" t="s">
-        <v>940</v>
+        <v>947</v>
       </c>
       <c r="K279">
         <v>0</v>
@@ -13646,13 +13688,13 @@
     </row>
     <row r="280" spans="1:11">
       <c r="A280" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
       <c r="B280" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="C280" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="D280">
         <v>1</v>
@@ -13681,13 +13723,13 @@
     </row>
     <row r="281" spans="1:11">
       <c r="A281" t="s">
-        <v>943</v>
+        <v>950</v>
       </c>
       <c r="B281" t="s">
-        <v>944</v>
+        <v>951</v>
       </c>
       <c r="C281" t="s">
-        <v>944</v>
+        <v>951</v>
       </c>
       <c r="D281">
         <v>1</v>
@@ -13716,13 +13758,13 @@
     </row>
     <row r="282" spans="1:11">
       <c r="A282" t="s">
-        <v>945</v>
+        <v>952</v>
       </c>
       <c r="B282" t="s">
-        <v>946</v>
+        <v>953</v>
       </c>
       <c r="C282" t="s">
-        <v>946</v>
+        <v>953</v>
       </c>
       <c r="D282">
         <v>1</v>
@@ -13751,13 +13793,13 @@
     </row>
     <row r="283" spans="1:11">
       <c r="A283" t="s">
-        <v>947</v>
+        <v>954</v>
       </c>
       <c r="B283" t="s">
-        <v>948</v>
+        <v>955</v>
       </c>
       <c r="C283" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -13769,7 +13811,7 @@
         <v>0.16107144603648099</v>
       </c>
       <c r="G283" t="s">
-        <v>950</v>
+        <v>957</v>
       </c>
       <c r="H283">
         <v>0.15</v>
@@ -13778,7 +13820,7 @@
         <v>8.2400000000000001E-2</v>
       </c>
       <c r="J283" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -13786,13 +13828,13 @@
     </row>
     <row r="284" spans="1:11">
       <c r="A284" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
       <c r="B284" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
       <c r="C284" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -13804,7 +13846,7 @@
         <v>0.99985185185185188</v>
       </c>
       <c r="G284" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
       <c r="H284">
         <v>0.92</v>
@@ -13821,13 +13863,13 @@
     </row>
     <row r="285" spans="1:11">
       <c r="A285" t="s">
-        <v>956</v>
+        <v>963</v>
       </c>
       <c r="B285" t="s">
-        <v>957</v>
+        <v>964</v>
       </c>
       <c r="C285" t="s">
-        <v>958</v>
+        <v>965</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -13839,7 +13881,7 @@
         <v>0.99999088788453128</v>
       </c>
       <c r="G285" t="s">
-        <v>959</v>
+        <v>966</v>
       </c>
       <c r="H285">
         <v>1</v>
@@ -13856,13 +13898,13 @@
     </row>
     <row r="286" spans="1:11">
       <c r="A286" t="s">
-        <v>960</v>
+        <v>967</v>
       </c>
       <c r="B286" t="s">
-        <v>961</v>
+        <v>968</v>
       </c>
       <c r="C286" t="s">
-        <v>962</v>
+        <v>969</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -13874,7 +13916,7 @@
         <v>0.40546209674036149</v>
       </c>
       <c r="G286" t="s">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="H286">
         <v>0.21</v>
@@ -13883,7 +13925,7 @@
         <v>0.58109999999999995</v>
       </c>
       <c r="J286" t="s">
-        <v>964</v>
+        <v>971</v>
       </c>
       <c r="K286">
         <v>0</v>
@@ -13891,13 +13933,13 @@
     </row>
     <row r="287" spans="1:11">
       <c r="A287" t="s">
-        <v>965</v>
+        <v>972</v>
       </c>
       <c r="B287" t="s">
-        <v>966</v>
+        <v>973</v>
       </c>
       <c r="C287" t="s">
-        <v>966</v>
+        <v>973</v>
       </c>
       <c r="D287">
         <v>1</v>
@@ -13926,13 +13968,13 @@
     </row>
     <row r="288" spans="1:11">
       <c r="A288" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
       <c r="B288" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="C288" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="D288">
         <v>1</v>
@@ -13961,13 +14003,13 @@
     </row>
     <row r="289" spans="1:11">
       <c r="A289" t="s">
-        <v>969</v>
+        <v>976</v>
       </c>
       <c r="B289" t="s">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="C289" t="s">
-        <v>971</v>
+        <v>978</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -13979,7 +14021,7 @@
         <v>0.99999451303155007</v>
       </c>
       <c r="G289" t="s">
-        <v>972</v>
+        <v>979</v>
       </c>
       <c r="H289">
         <v>0.92</v>
@@ -13988,7 +14030,7 @@
         <v>0.98659999999999992</v>
       </c>
       <c r="J289" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -13996,13 +14038,13 @@
     </row>
     <row r="290" spans="1:11">
       <c r="A290" t="s">
-        <v>974</v>
+        <v>981</v>
       </c>
       <c r="B290" t="s">
-        <v>975</v>
+        <v>982</v>
       </c>
       <c r="C290" t="s">
-        <v>975</v>
+        <v>982</v>
       </c>
       <c r="D290">
         <v>1</v>
@@ -14031,13 +14073,13 @@
     </row>
     <row r="291" spans="1:11">
       <c r="A291" t="s">
-        <v>976</v>
+        <v>983</v>
       </c>
       <c r="B291" t="s">
-        <v>977</v>
+        <v>984</v>
       </c>
       <c r="C291" t="s">
-        <v>977</v>
+        <v>984</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -14066,13 +14108,13 @@
     </row>
     <row r="292" spans="1:11">
       <c r="A292" t="s">
-        <v>978</v>
+        <v>985</v>
       </c>
       <c r="B292" t="s">
-        <v>979</v>
+        <v>986</v>
       </c>
       <c r="C292" t="s">
-        <v>980</v>
+        <v>987</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -14084,7 +14126,7 @@
         <v>0.93487490844375576</v>
       </c>
       <c r="G292" t="s">
-        <v>981</v>
+        <v>988</v>
       </c>
       <c r="H292">
         <v>0.9</v>
@@ -14093,7 +14135,7 @@
         <v>0.9909</v>
       </c>
       <c r="J292" t="s">
-        <v>982</v>
+        <v>989</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -14101,13 +14143,13 @@
     </row>
     <row r="293" spans="1:11">
       <c r="A293" t="s">
-        <v>983</v>
+        <v>990</v>
       </c>
       <c r="B293" t="s">
-        <v>984</v>
+        <v>991</v>
       </c>
       <c r="C293" t="s">
-        <v>984</v>
+        <v>991</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -14136,13 +14178,13 @@
     </row>
     <row r="294" spans="1:11">
       <c r="A294" t="s">
-        <v>985</v>
+        <v>992</v>
       </c>
       <c r="B294" t="s">
-        <v>986</v>
+        <v>993</v>
       </c>
       <c r="C294" t="s">
-        <v>987</v>
+        <v>994</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -14154,7 +14196,7 @@
         <v>0.70304985209989224</v>
       </c>
       <c r="G294" t="s">
-        <v>988</v>
+        <v>995</v>
       </c>
       <c r="H294">
         <v>0.66</v>
@@ -14163,7 +14205,7 @@
         <v>0.97909999999999997</v>
       </c>
       <c r="J294" t="s">
-        <v>989</v>
+        <v>996</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -14171,13 +14213,13 @@
     </row>
     <row r="295" spans="1:11">
       <c r="A295" t="s">
-        <v>990</v>
+        <v>997</v>
       </c>
       <c r="B295" t="s">
-        <v>991</v>
+        <v>998</v>
       </c>
       <c r="C295" t="s">
-        <v>992</v>
+        <v>999</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -14189,7 +14231,7 @@
         <v>0.99999902343750002</v>
       </c>
       <c r="G295" t="s">
-        <v>993</v>
+        <v>1000</v>
       </c>
       <c r="H295">
         <v>1</v>
@@ -14198,7 +14240,7 @@
         <v>1</v>
       </c>
       <c r="J295" t="s">
-        <v>994</v>
+        <v>1001</v>
       </c>
       <c r="K295">
         <v>0</v>
@@ -14206,13 +14248,13 @@
     </row>
     <row r="296" spans="1:11">
       <c r="A296" t="s">
-        <v>995</v>
+        <v>1002</v>
       </c>
       <c r="B296" t="s">
-        <v>996</v>
+        <v>1003</v>
       </c>
       <c r="C296" t="s">
-        <v>997</v>
+        <v>1004</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -14224,7 +14266,7 @@
         <v>0.99999518411142041</v>
       </c>
       <c r="G296" t="s">
-        <v>998</v>
+        <v>1005</v>
       </c>
       <c r="H296">
         <v>1</v>
@@ -14233,7 +14275,7 @@
         <v>1</v>
       </c>
       <c r="J296" t="s">
-        <v>999</v>
+        <v>1006</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -14241,13 +14283,13 @@
     </row>
     <row r="297" spans="1:11">
       <c r="A297" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
       <c r="B297" t="s">
-        <v>1001</v>
+        <v>1008</v>
       </c>
       <c r="C297" t="s">
-        <v>1001</v>
+        <v>1008</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -14276,13 +14318,13 @@
     </row>
     <row r="298" spans="1:11">
       <c r="A298" t="s">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="B298" t="s">
-        <v>1003</v>
+        <v>1010</v>
       </c>
       <c r="C298" t="s">
-        <v>1004</v>
+        <v>1011</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -14294,7 +14336,7 @@
         <v>0.96253492767915849</v>
       </c>
       <c r="G298" t="s">
-        <v>1005</v>
+        <v>1012</v>
       </c>
       <c r="H298">
         <v>0.83</v>
@@ -14303,7 +14345,7 @@
         <v>0.9484999999999999</v>
       </c>
       <c r="J298" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -14311,13 +14353,13 @@
     </row>
     <row r="299" spans="1:11">
       <c r="A299" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
       <c r="B299" t="s">
-        <v>1008</v>
+        <v>1015</v>
       </c>
       <c r="C299" t="s">
-        <v>1008</v>
+        <v>1015</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -14346,13 +14388,13 @@
     </row>
     <row r="300" spans="1:11">
       <c r="A300" t="s">
-        <v>1009</v>
+        <v>1016</v>
       </c>
       <c r="B300" t="s">
-        <v>1010</v>
+        <v>1017</v>
       </c>
       <c r="C300" t="s">
-        <v>1011</v>
+        <v>1018</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -14364,7 +14406,7 @@
         <v>0.96831509702158602</v>
       </c>
       <c r="G300" t="s">
-        <v>1012</v>
+        <v>1019</v>
       </c>
       <c r="H300">
         <v>0.69</v>
@@ -14373,7 +14415,7 @@
         <v>0.87959999999999994</v>
       </c>
       <c r="J300" t="s">
-        <v>982</v>
+        <v>989</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -14381,13 +14423,13 @@
     </row>
     <row r="301" spans="1:11">
       <c r="A301" t="s">
-        <v>1013</v>
+        <v>1020</v>
       </c>
       <c r="B301" t="s">
-        <v>1014</v>
+        <v>1021</v>
       </c>
       <c r="C301" t="s">
-        <v>1014</v>
+        <v>1021</v>
       </c>
       <c r="D301">
         <v>1</v>
@@ -14416,13 +14458,13 @@
     </row>
     <row r="302" spans="1:11">
       <c r="A302" t="s">
-        <v>1015</v>
+        <v>1022</v>
       </c>
       <c r="B302" t="s">
-        <v>1016</v>
+        <v>1023</v>
       </c>
       <c r="C302" t="s">
-        <v>1017</v>
+        <v>1024</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -14434,7 +14476,7 @@
         <v>0.999996</v>
       </c>
       <c r="G302" t="s">
-        <v>1018</v>
+        <v>1025</v>
       </c>
       <c r="H302">
         <v>1</v>
@@ -14443,7 +14485,7 @@
         <v>1</v>
       </c>
       <c r="J302" t="s">
-        <v>1019</v>
+        <v>1026</v>
       </c>
       <c r="K302">
         <v>0</v>
@@ -14451,13 +14493,13 @@
     </row>
     <row r="303" spans="1:11">
       <c r="A303" t="s">
-        <v>1020</v>
+        <v>1027</v>
       </c>
       <c r="B303" t="s">
-        <v>1021</v>
+        <v>1028</v>
       </c>
       <c r="C303" t="s">
-        <v>1022</v>
+        <v>1029</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -14469,7 +14511,7 @@
         <v>0.74476011756102278</v>
       </c>
       <c r="G303" t="s">
-        <v>1023</v>
+        <v>1030</v>
       </c>
       <c r="H303">
         <v>0.56000000000000005</v>
@@ -14478,7 +14520,7 @@
         <v>0.76290000000000002</v>
       </c>
       <c r="J303" t="s">
-        <v>1024</v>
+        <v>1031</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -14486,13 +14528,13 @@
     </row>
     <row r="304" spans="1:11">
       <c r="A304" t="s">
-        <v>1025</v>
+        <v>1032</v>
       </c>
       <c r="B304" t="s">
-        <v>1026</v>
+        <v>1033</v>
       </c>
       <c r="C304" t="s">
-        <v>1027</v>
+        <v>1034</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -14504,7 +14546,7 @@
         <v>0.64379423183166962</v>
       </c>
       <c r="G304" t="s">
-        <v>1028</v>
+        <v>1035</v>
       </c>
       <c r="H304">
         <v>0.56999999999999995</v>
@@ -14513,7 +14555,7 @@
         <v>0.93209999999999993</v>
       </c>
       <c r="J304" t="s">
-        <v>1029</v>
+        <v>1036</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -14521,13 +14563,13 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305" t="s">
-        <v>1030</v>
+        <v>1037</v>
       </c>
       <c r="B305" t="s">
-        <v>1031</v>
+        <v>1038</v>
       </c>
       <c r="C305" t="s">
-        <v>1031</v>
+        <v>1038</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -14556,13 +14598,13 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306" t="s">
-        <v>1032</v>
+        <v>1039</v>
       </c>
       <c r="B306" t="s">
-        <v>1033</v>
+        <v>1040</v>
       </c>
       <c r="C306" t="s">
-        <v>1034</v>
+        <v>1041</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -14574,7 +14616,7 @@
         <v>0.97417177571210234</v>
       </c>
       <c r="G306" t="s">
-        <v>1035</v>
+        <v>1042</v>
       </c>
       <c r="H306">
         <v>0.93</v>
@@ -14583,7 +14625,7 @@
         <v>0.98209999999999997</v>
       </c>
       <c r="J306" t="s">
-        <v>1036</v>
+        <v>1043</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -14591,13 +14633,13 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307" t="s">
-        <v>1037</v>
+        <v>1044</v>
       </c>
       <c r="B307" t="s">
-        <v>1038</v>
+        <v>1045</v>
       </c>
       <c r="C307" t="s">
-        <v>1038</v>
+        <v>1045</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -14626,13 +14668,13 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308" t="s">
-        <v>1039</v>
+        <v>1046</v>
       </c>
       <c r="B308" t="s">
-        <v>1040</v>
+        <v>1047</v>
       </c>
       <c r="C308" t="s">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -14644,7 +14686,7 @@
         <v>0.98664022774046589</v>
       </c>
       <c r="G308" t="s">
-        <v>1042</v>
+        <v>1049</v>
       </c>
       <c r="H308">
         <v>0.97</v>
@@ -14653,7 +14695,7 @@
         <v>0.98909999999999998</v>
       </c>
       <c r="J308" t="s">
-        <v>1043</v>
+        <v>1050</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -14661,13 +14703,13 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309" t="s">
-        <v>1044</v>
+        <v>1051</v>
       </c>
       <c r="B309" t="s">
-        <v>1045</v>
+        <v>1052</v>
       </c>
       <c r="C309" t="s">
-        <v>1046</v>
+        <v>1053</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -14679,7 +14721,7 @@
         <v>0.99995890523547304</v>
       </c>
       <c r="G309" t="s">
-        <v>1047</v>
+        <v>1054</v>
       </c>
       <c r="H309">
         <v>1</v>
@@ -14688,7 +14730,7 @@
         <v>1</v>
       </c>
       <c r="J309" t="s">
-        <v>940</v>
+        <v>947</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -14696,13 +14738,13 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310" t="s">
-        <v>1048</v>
+        <v>1055</v>
       </c>
       <c r="B310" t="s">
-        <v>1049</v>
+        <v>1056</v>
       </c>
       <c r="C310" t="s">
-        <v>1049</v>
+        <v>1056</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -14731,13 +14773,13 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311" t="s">
-        <v>1050</v>
+        <v>1057</v>
       </c>
       <c r="B311" t="s">
-        <v>1051</v>
+        <v>1058</v>
       </c>
       <c r="C311" t="s">
-        <v>1052</v>
+        <v>1059</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -14749,7 +14791,7 @@
         <v>0.99998928326474623</v>
       </c>
       <c r="G311" t="s">
-        <v>1053</v>
+        <v>1060</v>
       </c>
       <c r="H311">
         <v>1</v>
@@ -14766,13 +14808,13 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312" t="s">
-        <v>1054</v>
+        <v>1061</v>
       </c>
       <c r="B312" t="s">
-        <v>1055</v>
+        <v>1062</v>
       </c>
       <c r="C312" t="s">
-        <v>1056</v>
+        <v>1063</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -14784,7 +14826,7 @@
         <v>0.97341886358453711</v>
       </c>
       <c r="G312" t="s">
-        <v>1057</v>
+        <v>1064</v>
       </c>
       <c r="H312">
         <v>0.94</v>
@@ -14793,7 +14835,7 @@
         <v>0.97719999999999996</v>
       </c>
       <c r="J312" t="s">
-        <v>1058</v>
+        <v>1065</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -14801,13 +14843,13 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313" t="s">
-        <v>1059</v>
+        <v>1066</v>
       </c>
       <c r="B313" t="s">
-        <v>1060</v>
+        <v>1067</v>
       </c>
       <c r="C313" t="s">
-        <v>1061</v>
+        <v>1068</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -14819,7 +14861,7 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313" t="s">
-        <v>1062</v>
+        <v>1069</v>
       </c>
       <c r="H313">
         <v>0.89</v>
@@ -14828,7 +14870,7 @@
         <v>0.9756999999999999</v>
       </c>
       <c r="J313" t="s">
-        <v>1063</v>
+        <v>1070</v>
       </c>
       <c r="K313">
         <v>0</v>
@@ -14836,13 +14878,13 @@
     </row>
     <row r="314" spans="1:11">
       <c r="A314" t="s">
-        <v>1064</v>
+        <v>1071</v>
       </c>
       <c r="B314" t="s">
-        <v>1065</v>
+        <v>1072</v>
       </c>
       <c r="C314" t="s">
-        <v>1066</v>
+        <v>1073</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -14854,7 +14896,7 @@
         <v>0.75858170895276666</v>
       </c>
       <c r="G314" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="H314">
         <v>0.54</v>
@@ -14863,7 +14905,7 @@
         <v>0.68030000000000002</v>
       </c>
       <c r="J314" t="s">
-        <v>1068</v>
+        <v>1075</v>
       </c>
       <c r="K314">
         <v>0</v>
@@ -14871,13 +14913,13 @@
     </row>
     <row r="315" spans="1:11">
       <c r="A315" t="s">
-        <v>1069</v>
+        <v>1076</v>
       </c>
       <c r="B315" t="s">
-        <v>1070</v>
+        <v>1077</v>
       </c>
       <c r="C315" t="s">
-        <v>1071</v>
+        <v>1078</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -14889,7 +14931,7 @@
         <v>0.998317618783509</v>
       </c>
       <c r="G315" t="s">
-        <v>1072</v>
+        <v>1079</v>
       </c>
       <c r="H315">
         <v>0.9</v>
@@ -14898,7 +14940,7 @@
         <v>0.97470000000000001</v>
       </c>
       <c r="J315" t="s">
-        <v>1073</v>
+        <v>1080</v>
       </c>
       <c r="K315">
         <v>0</v>
@@ -14906,13 +14948,13 @@
     </row>
     <row r="316" spans="1:11">
       <c r="A316" t="s">
-        <v>1074</v>
+        <v>1081</v>
       </c>
       <c r="B316" t="s">
-        <v>1075</v>
+        <v>1082</v>
       </c>
       <c r="C316" t="s">
-        <v>1076</v>
+        <v>1083</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -14924,7 +14966,7 @@
         <v>0.95598287878305699</v>
       </c>
       <c r="G316" t="s">
-        <v>1077</v>
+        <v>1084</v>
       </c>
       <c r="H316">
         <v>0.92</v>
@@ -14933,7 +14975,7 @@
         <v>0.97089999999999999</v>
       </c>
       <c r="J316" t="s">
-        <v>1078</v>
+        <v>1085</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -14941,13 +14983,13 @@
     </row>
     <row r="317" spans="1:11">
       <c r="A317" t="s">
-        <v>1079</v>
+        <v>1086</v>
       </c>
       <c r="B317" t="s">
-        <v>1080</v>
+        <v>1087</v>
       </c>
       <c r="C317" t="s">
-        <v>1080</v>
+        <v>1087</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -14976,13 +15018,13 @@
     </row>
     <row r="318" spans="1:11">
       <c r="A318" t="s">
-        <v>1081</v>
+        <v>1088</v>
       </c>
       <c r="B318" t="s">
-        <v>1082</v>
+        <v>1089</v>
       </c>
       <c r="C318" t="s">
-        <v>1083</v>
+        <v>1090</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -14994,7 +15036,7 @@
         <v>0.95178740438847254</v>
       </c>
       <c r="G318" t="s">
-        <v>1084</v>
+        <v>1091</v>
       </c>
       <c r="H318">
         <v>0.9</v>
@@ -15003,7 +15045,7 @@
         <v>0.97430000000000005</v>
       </c>
       <c r="J318" t="s">
-        <v>1085</v>
+        <v>1092</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -15011,13 +15053,13 @@
     </row>
     <row r="319" spans="1:11">
       <c r="A319" t="s">
-        <v>1086</v>
+        <v>1093</v>
       </c>
       <c r="B319" t="s">
-        <v>1087</v>
+        <v>1094</v>
       </c>
       <c r="C319" t="s">
-        <v>1088</v>
+        <v>1095</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -15029,7 +15071,7 @@
         <v>0.70336391437308876</v>
       </c>
       <c r="G319" t="s">
-        <v>1089</v>
+        <v>1096</v>
       </c>
       <c r="H319">
         <v>0.41</v>
@@ -15038,7 +15080,7 @@
         <v>0.80920000000000003</v>
       </c>
       <c r="J319" t="s">
-        <v>1090</v>
+        <v>1097</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -15046,13 +15088,13 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320" t="s">
-        <v>1091</v>
+        <v>1098</v>
       </c>
       <c r="B320" t="s">
-        <v>1092</v>
+        <v>1099</v>
       </c>
       <c r="C320" t="s">
-        <v>1092</v>
+        <v>1099</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -15081,13 +15123,13 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1093</v>
+        <v>1100</v>
       </c>
       <c r="B321" t="s">
-        <v>1094</v>
+        <v>1101</v>
       </c>
       <c r="C321" t="s">
-        <v>1095</v>
+        <v>1102</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -15099,7 +15141,7 @@
         <v>0.99849640734645617</v>
       </c>
       <c r="G321" t="s">
-        <v>1096</v>
+        <v>1103</v>
       </c>
       <c r="H321">
         <v>0.98</v>
@@ -15108,7 +15150,7 @@
         <v>0.99470000000000003</v>
       </c>
       <c r="J321" t="s">
-        <v>1097</v>
+        <v>1104</v>
       </c>
       <c r="K321">
         <v>0</v>
@@ -15116,13 +15158,13 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1098</v>
+        <v>1105</v>
       </c>
       <c r="B322" t="s">
-        <v>1099</v>
+        <v>1106</v>
       </c>
       <c r="C322" t="s">
-        <v>1099</v>
+        <v>1106</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -15151,13 +15193,13 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1100</v>
+        <v>1107</v>
       </c>
       <c r="B323" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
       <c r="C323" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -15186,13 +15228,13 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1102</v>
+        <v>1109</v>
       </c>
       <c r="B324" t="s">
-        <v>1103</v>
+        <v>1110</v>
       </c>
       <c r="C324" t="s">
-        <v>1104</v>
+        <v>1111</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -15204,7 +15246,7 @@
         <v>0.99690437876548454</v>
       </c>
       <c r="G324" t="s">
-        <v>1105</v>
+        <v>1112</v>
       </c>
       <c r="H324">
         <v>0.95</v>
@@ -15213,7 +15255,7 @@
         <v>0.98730000000000007</v>
       </c>
       <c r="J324" t="s">
-        <v>1106</v>
+        <v>1113</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -15221,13 +15263,13 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1107</v>
+        <v>1114</v>
       </c>
       <c r="B325" t="s">
-        <v>1108</v>
+        <v>1115</v>
       </c>
       <c r="C325" t="s">
-        <v>1109</v>
+        <v>1116</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -15239,7 +15281,7 @@
         <v>0.9999968246710359</v>
       </c>
       <c r="G325" t="s">
-        <v>1110</v>
+        <v>1117</v>
       </c>
       <c r="H325">
         <v>1</v>
@@ -15248,7 +15290,7 @@
         <v>1</v>
       </c>
       <c r="J325" t="s">
-        <v>1111</v>
+        <v>1118</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -15256,13 +15298,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1112</v>
+        <v>1119</v>
       </c>
       <c r="B326" t="s">
-        <v>1113</v>
+        <v>1120</v>
       </c>
       <c r="C326" t="s">
-        <v>1113</v>
+        <v>1120</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -15291,13 +15333,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1114</v>
+        <v>1121</v>
       </c>
       <c r="B327" t="s">
-        <v>1115</v>
+        <v>1122</v>
       </c>
       <c r="C327" t="s">
-        <v>1115</v>
+        <v>1122</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Aggiunte ulteriori valutazione CodeT5_770
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/Analisi_CodeT5_770.xlsx
+++ b/HE/W_in_progress/Analisi_CodeT5_770.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F32A0078-DD93-4352-B664-98BE0AB71245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28AAE9D6-7468-456B-BAC8-51747266CC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="1131">
   <si>
     <t>IN</t>
   </si>
@@ -2550,6 +2550,9 @@
     <t>0.2448979542357352</t>
   </si>
   <si>
+    <t>Non è un priority encoder</t>
+  </si>
+  <si>
     <t>Define a ring counter of N-bit with the signals clock and reset as input and the signal ring_count (N-bit) as output.</t>
   </si>
   <si>
@@ -2565,6 +2568,9 @@
     <t>0.4955752162487274</t>
   </si>
   <si>
+    <t>Non è un ring counter</t>
+  </si>
+  <si>
     <t>Implement a binary to BCD converter</t>
   </si>
   <si>
@@ -2580,6 +2586,9 @@
     <t>0.6019417426788577</t>
   </si>
   <si>
+    <t>Non esegue una conversione BCD</t>
+  </si>
+  <si>
     <t>Create a pulse generator that outputs a single pulse every N clock cycles</t>
   </si>
   <si>
@@ -2595,6 +2604,9 @@
     <t>0.7628865929386759</t>
   </si>
   <si>
+    <t>Fa robe strane</t>
+  </si>
+  <si>
     <t>Define a binary to BCD converter of (N/3)+1-digit with the signal binary_value (N-bit) as input and the signal BCD_value ((N/3)+1-digit) as output.</t>
   </si>
   <si>
@@ -2622,6 +2634,9 @@
     <t>0.7480915980886895</t>
   </si>
   <si>
+    <t xml:space="preserve">Errori sintattici, ma ci può stare </t>
+  </si>
+  <si>
     <t>Generate a dual-port memory of K x L with the signals clock, write, address_w (log2K-bit), address_r (log2K-bit), and data_write (L-bit) as input and the signal data_read (L-bit) as output.</t>
   </si>
   <si>
@@ -2637,6 +2652,9 @@
     <t>0.46031745532879825</t>
   </si>
   <si>
+    <t>Più o meno</t>
+  </si>
+  <si>
     <t>Create a 4-bit binary counter that increments on each clock pulse and resets asynchronously</t>
   </si>
   <si>
@@ -2667,6 +2685,9 @@
     <t>0.5517241329502974</t>
   </si>
   <si>
+    <t>Non proprio un Filtro FIR</t>
+  </si>
+  <si>
     <t>Implement a basic clock gating circuit</t>
   </si>
   <si>
@@ -2680,6 +2701,9 @@
   </si>
   <si>
     <t>0.25806451175858486</t>
+  </si>
+  <si>
+    <t>Non un clock gating circuit</t>
   </si>
   <si>
     <t>Write a floating-point multiplier of N-bit with the signals A (N-bit) and B (N-bit) as input and the signal product (N-bit) as output.</t>
@@ -3772,8 +3796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="K256" sqref="K256"/>
+    <sheetView tabSelected="1" topLeftCell="C244" workbookViewId="0">
+      <selection activeCell="L266" sqref="L266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3784,10 +3808,10 @@
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" customWidth="1"/>
     <col min="9" max="9" width="8.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="37.85546875" customWidth="1"/>
   </cols>
@@ -12880,16 +12904,19 @@
       <c r="K256">
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:11">
+      <c r="L256" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
       <c r="A257" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B257" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C257" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -12901,7 +12928,7 @@
         <v>0.52996093454314475</v>
       </c>
       <c r="G257" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="H257">
         <v>0</v>
@@ -12910,21 +12937,24 @@
         <v>0.86849999999999994</v>
       </c>
       <c r="J257" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="K257">
         <v>0</v>
       </c>
-    </row>
-    <row r="258" spans="1:11">
+      <c r="L257" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
       <c r="A258" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B258" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="C258" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -12936,7 +12966,7 @@
         <v>0.33777001839693588</v>
       </c>
       <c r="G258" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="H258">
         <v>0.11</v>
@@ -12945,21 +12975,24 @@
         <v>0.87250000000000005</v>
       </c>
       <c r="J258" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="K258">
         <v>0</v>
       </c>
-    </row>
-    <row r="259" spans="1:11">
+      <c r="L258" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
       <c r="A259" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="B259" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="C259" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -12971,7 +13004,7 @@
         <v>0.70155685702998627</v>
       </c>
       <c r="G259" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="H259">
         <v>0.38</v>
@@ -12980,21 +13013,24 @@
         <v>0.89639999999999997</v>
       </c>
       <c r="J259" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="K259">
         <v>0</v>
       </c>
-    </row>
-    <row r="260" spans="1:11">
+      <c r="L259" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12">
       <c r="A260" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="B260" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="C260" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -13006,7 +13042,7 @@
         <v>0.6247741645144721</v>
       </c>
       <c r="G260" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="H260">
         <v>0.63</v>
@@ -13018,18 +13054,18 @@
         <v>429</v>
       </c>
       <c r="K260">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12">
       <c r="A261" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="B261" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="C261" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -13041,7 +13077,7 @@
         <v>0.61378041019317575</v>
       </c>
       <c r="G261" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="H261">
         <v>0.47</v>
@@ -13050,21 +13086,24 @@
         <v>0.84250000000000003</v>
       </c>
       <c r="J261" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="K261">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L261" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12">
       <c r="A262" t="s">
-        <v>863</v>
+        <v>868</v>
       </c>
       <c r="B262" t="s">
-        <v>864</v>
+        <v>869</v>
       </c>
       <c r="C262" t="s">
-        <v>865</v>
+        <v>870</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -13076,7 +13115,7 @@
         <v>0.68835513277843841</v>
       </c>
       <c r="G262" t="s">
-        <v>866</v>
+        <v>871</v>
       </c>
       <c r="H262">
         <v>0.26</v>
@@ -13085,21 +13124,24 @@
         <v>0.80209999999999992</v>
       </c>
       <c r="J262" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
       <c r="K262">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L262" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12">
       <c r="A263" t="s">
-        <v>868</v>
+        <v>874</v>
       </c>
       <c r="B263" t="s">
-        <v>869</v>
+        <v>875</v>
       </c>
       <c r="C263" t="s">
-        <v>870</v>
+        <v>876</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -13111,7 +13153,7 @@
         <v>0.93440094834565979</v>
       </c>
       <c r="G263" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="H263">
         <v>0</v>
@@ -13120,21 +13162,21 @@
         <v>0.90010000000000001</v>
       </c>
       <c r="J263" t="s">
-        <v>872</v>
+        <v>878</v>
       </c>
       <c r="K263">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12">
       <c r="A264" t="s">
-        <v>873</v>
+        <v>879</v>
       </c>
       <c r="B264" t="s">
-        <v>874</v>
+        <v>880</v>
       </c>
       <c r="C264" t="s">
-        <v>875</v>
+        <v>881</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -13146,7 +13188,7 @@
         <v>0.52763364298887605</v>
       </c>
       <c r="G264" t="s">
-        <v>876</v>
+        <v>882</v>
       </c>
       <c r="H264">
         <v>0</v>
@@ -13155,21 +13197,24 @@
         <v>0.87620000000000009</v>
       </c>
       <c r="J264" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="K264">
         <v>0</v>
       </c>
-    </row>
-    <row r="265" spans="1:11">
+      <c r="L264" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12">
       <c r="A265" t="s">
-        <v>878</v>
+        <v>885</v>
       </c>
       <c r="B265" t="s">
-        <v>879</v>
+        <v>886</v>
       </c>
       <c r="C265" t="s">
-        <v>880</v>
+        <v>887</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -13181,7 +13226,7 @@
         <v>0.50355774493705519</v>
       </c>
       <c r="G265" t="s">
-        <v>881</v>
+        <v>888</v>
       </c>
       <c r="H265">
         <v>0</v>
@@ -13190,21 +13235,24 @@
         <v>0.67669999999999997</v>
       </c>
       <c r="J265" t="s">
-        <v>882</v>
+        <v>889</v>
       </c>
       <c r="K265">
         <v>0</v>
       </c>
-    </row>
-    <row r="266" spans="1:11">
+      <c r="L265" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12">
       <c r="A266" t="s">
-        <v>883</v>
+        <v>891</v>
       </c>
       <c r="B266" t="s">
-        <v>884</v>
+        <v>892</v>
       </c>
       <c r="C266" t="s">
-        <v>885</v>
+        <v>893</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -13216,7 +13264,7 @@
         <v>0.52121822842574161</v>
       </c>
       <c r="G266" t="s">
-        <v>886</v>
+        <v>894</v>
       </c>
       <c r="H266">
         <v>0.17</v>
@@ -13225,21 +13273,21 @@
         <v>0.89410000000000001</v>
       </c>
       <c r="J266" t="s">
-        <v>887</v>
+        <v>895</v>
       </c>
       <c r="K266">
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:11">
+    <row r="267" spans="1:12">
       <c r="A267" t="s">
-        <v>888</v>
+        <v>896</v>
       </c>
       <c r="B267" t="s">
-        <v>889</v>
+        <v>897</v>
       </c>
       <c r="C267" t="s">
-        <v>890</v>
+        <v>898</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -13251,7 +13299,7 @@
         <v>0.24464916656274679</v>
       </c>
       <c r="G267" t="s">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="H267">
         <v>0.14000000000000001</v>
@@ -13260,21 +13308,21 @@
         <v>0.96260000000000001</v>
       </c>
       <c r="J267" t="s">
-        <v>892</v>
+        <v>900</v>
       </c>
       <c r="K267">
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:11">
+    <row r="268" spans="1:12">
       <c r="A268" t="s">
-        <v>893</v>
+        <v>901</v>
       </c>
       <c r="B268" t="s">
-        <v>894</v>
+        <v>902</v>
       </c>
       <c r="C268" t="s">
-        <v>895</v>
+        <v>903</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -13286,7 +13334,7 @@
         <v>0.42987585923874011</v>
       </c>
       <c r="G268" t="s">
-        <v>896</v>
+        <v>904</v>
       </c>
       <c r="H268">
         <v>0</v>
@@ -13295,21 +13343,21 @@
         <v>0.9335</v>
       </c>
       <c r="J268" t="s">
-        <v>897</v>
+        <v>905</v>
       </c>
       <c r="K268">
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:11">
+    <row r="269" spans="1:12">
       <c r="A269" t="s">
-        <v>898</v>
+        <v>906</v>
       </c>
       <c r="B269" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="C269" t="s">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -13321,7 +13369,7 @@
         <v>0.86196594368483526</v>
       </c>
       <c r="G269" t="s">
-        <v>901</v>
+        <v>909</v>
       </c>
       <c r="H269">
         <v>0.76</v>
@@ -13330,21 +13378,21 @@
         <v>0.94590000000000007</v>
       </c>
       <c r="J269" t="s">
-        <v>902</v>
+        <v>910</v>
       </c>
       <c r="K269">
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:11">
+    <row r="270" spans="1:12">
       <c r="A270" t="s">
-        <v>903</v>
+        <v>911</v>
       </c>
       <c r="B270" t="s">
-        <v>904</v>
+        <v>912</v>
       </c>
       <c r="C270" t="s">
-        <v>905</v>
+        <v>913</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -13356,7 +13404,7 @@
         <v>0.88802454698719147</v>
       </c>
       <c r="G270" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="H270">
         <v>0.73</v>
@@ -13365,21 +13413,21 @@
         <v>0.97549999999999992</v>
       </c>
       <c r="J270" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="K270">
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:11">
+    <row r="271" spans="1:12">
       <c r="A271" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="B271" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="C271" t="s">
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -13391,7 +13439,7 @@
         <v>0.58879799469651517</v>
       </c>
       <c r="G271" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="H271">
         <v>0.16</v>
@@ -13400,21 +13448,21 @@
         <v>0.85709999999999997</v>
       </c>
       <c r="J271" t="s">
-        <v>912</v>
+        <v>920</v>
       </c>
       <c r="K271">
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" spans="1:12">
       <c r="A272" t="s">
-        <v>913</v>
+        <v>921</v>
       </c>
       <c r="B272" t="s">
-        <v>914</v>
+        <v>922</v>
       </c>
       <c r="C272" t="s">
-        <v>915</v>
+        <v>923</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -13426,7 +13474,7 @@
         <v>0.66424709652589042</v>
       </c>
       <c r="G272" t="s">
-        <v>916</v>
+        <v>924</v>
       </c>
       <c r="H272">
         <v>0</v>
@@ -13435,7 +13483,7 @@
         <v>0.77150000000000007</v>
       </c>
       <c r="J272" t="s">
-        <v>917</v>
+        <v>925</v>
       </c>
       <c r="K272">
         <v>0</v>
@@ -13443,13 +13491,13 @@
     </row>
     <row r="273" spans="1:11">
       <c r="A273" t="s">
-        <v>918</v>
+        <v>926</v>
       </c>
       <c r="B273" t="s">
-        <v>919</v>
+        <v>927</v>
       </c>
       <c r="C273" t="s">
-        <v>920</v>
+        <v>928</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -13461,7 +13509,7 @@
         <v>0.52442395360121852</v>
       </c>
       <c r="G273" t="s">
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="H273">
         <v>0</v>
@@ -13470,7 +13518,7 @@
         <v>0.73470000000000002</v>
       </c>
       <c r="J273" t="s">
-        <v>922</v>
+        <v>930</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -13478,13 +13526,13 @@
     </row>
     <row r="274" spans="1:11">
       <c r="A274" t="s">
-        <v>923</v>
+        <v>931</v>
       </c>
       <c r="B274" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="C274" t="s">
-        <v>880</v>
+        <v>887</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -13496,7 +13544,7 @@
         <v>0.17054273168875969</v>
       </c>
       <c r="G274" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -13505,7 +13553,7 @@
         <v>0.67669999999999997</v>
       </c>
       <c r="J274" t="s">
-        <v>926</v>
+        <v>934</v>
       </c>
       <c r="K274">
         <v>0</v>
@@ -13513,13 +13561,13 @@
     </row>
     <row r="275" spans="1:11">
       <c r="A275" t="s">
-        <v>927</v>
+        <v>935</v>
       </c>
       <c r="B275" t="s">
-        <v>928</v>
+        <v>936</v>
       </c>
       <c r="C275" t="s">
-        <v>929</v>
+        <v>937</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -13531,7 +13579,7 @@
         <v>0.25958012686025911</v>
       </c>
       <c r="G275" t="s">
-        <v>930</v>
+        <v>938</v>
       </c>
       <c r="H275">
         <v>0</v>
@@ -13540,7 +13588,7 @@
         <v>0.79760000000000009</v>
       </c>
       <c r="J275" t="s">
-        <v>931</v>
+        <v>939</v>
       </c>
       <c r="K275">
         <v>0</v>
@@ -13548,13 +13596,13 @@
     </row>
     <row r="276" spans="1:11">
       <c r="A276" t="s">
-        <v>932</v>
+        <v>940</v>
       </c>
       <c r="B276" t="s">
-        <v>933</v>
+        <v>941</v>
       </c>
       <c r="C276" t="s">
-        <v>934</v>
+        <v>942</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -13566,7 +13614,7 @@
         <v>0.48741343083544247</v>
       </c>
       <c r="G276" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="H276">
         <v>0.52</v>
@@ -13575,7 +13623,7 @@
         <v>0.80959999999999999</v>
       </c>
       <c r="J276" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="K276">
         <v>0</v>
@@ -13583,13 +13631,13 @@
     </row>
     <row r="277" spans="1:11">
       <c r="A277" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="B277" t="s">
-        <v>938</v>
+        <v>946</v>
       </c>
       <c r="C277" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -13601,7 +13649,7 @@
         <v>0.89602265394280345</v>
       </c>
       <c r="G277" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
       <c r="H277">
         <v>0.77</v>
@@ -13618,13 +13666,13 @@
     </row>
     <row r="278" spans="1:11">
       <c r="A278" t="s">
-        <v>941</v>
+        <v>949</v>
       </c>
       <c r="B278" t="s">
-        <v>942</v>
+        <v>950</v>
       </c>
       <c r="C278" t="s">
-        <v>942</v>
+        <v>950</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -13653,13 +13701,13 @@
     </row>
     <row r="279" spans="1:11">
       <c r="A279" t="s">
-        <v>943</v>
+        <v>951</v>
       </c>
       <c r="B279" t="s">
-        <v>944</v>
+        <v>952</v>
       </c>
       <c r="C279" t="s">
-        <v>945</v>
+        <v>953</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -13671,7 +13719,7 @@
         <v>0.99997459736828731</v>
       </c>
       <c r="G279" t="s">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="H279">
         <v>1</v>
@@ -13680,7 +13728,7 @@
         <v>1</v>
       </c>
       <c r="J279" t="s">
-        <v>947</v>
+        <v>955</v>
       </c>
       <c r="K279">
         <v>0</v>
@@ -13688,13 +13736,13 @@
     </row>
     <row r="280" spans="1:11">
       <c r="A280" t="s">
-        <v>948</v>
+        <v>956</v>
       </c>
       <c r="B280" t="s">
-        <v>949</v>
+        <v>957</v>
       </c>
       <c r="C280" t="s">
-        <v>949</v>
+        <v>957</v>
       </c>
       <c r="D280">
         <v>1</v>
@@ -13723,13 +13771,13 @@
     </row>
     <row r="281" spans="1:11">
       <c r="A281" t="s">
-        <v>950</v>
+        <v>958</v>
       </c>
       <c r="B281" t="s">
-        <v>951</v>
+        <v>959</v>
       </c>
       <c r="C281" t="s">
-        <v>951</v>
+        <v>959</v>
       </c>
       <c r="D281">
         <v>1</v>
@@ -13758,13 +13806,13 @@
     </row>
     <row r="282" spans="1:11">
       <c r="A282" t="s">
-        <v>952</v>
+        <v>960</v>
       </c>
       <c r="B282" t="s">
-        <v>953</v>
+        <v>961</v>
       </c>
       <c r="C282" t="s">
-        <v>953</v>
+        <v>961</v>
       </c>
       <c r="D282">
         <v>1</v>
@@ -13793,13 +13841,13 @@
     </row>
     <row r="283" spans="1:11">
       <c r="A283" t="s">
-        <v>954</v>
+        <v>962</v>
       </c>
       <c r="B283" t="s">
-        <v>955</v>
+        <v>963</v>
       </c>
       <c r="C283" t="s">
-        <v>956</v>
+        <v>964</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -13811,7 +13859,7 @@
         <v>0.16107144603648099</v>
       </c>
       <c r="G283" t="s">
-        <v>957</v>
+        <v>965</v>
       </c>
       <c r="H283">
         <v>0.15</v>
@@ -13820,7 +13868,7 @@
         <v>8.2400000000000001E-2</v>
       </c>
       <c r="J283" t="s">
-        <v>958</v>
+        <v>966</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -13828,13 +13876,13 @@
     </row>
     <row r="284" spans="1:11">
       <c r="A284" t="s">
-        <v>959</v>
+        <v>967</v>
       </c>
       <c r="B284" t="s">
-        <v>960</v>
+        <v>968</v>
       </c>
       <c r="C284" t="s">
-        <v>961</v>
+        <v>969</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -13846,7 +13894,7 @@
         <v>0.99985185185185188</v>
       </c>
       <c r="G284" t="s">
-        <v>962</v>
+        <v>970</v>
       </c>
       <c r="H284">
         <v>0.92</v>
@@ -13863,13 +13911,13 @@
     </row>
     <row r="285" spans="1:11">
       <c r="A285" t="s">
-        <v>963</v>
+        <v>971</v>
       </c>
       <c r="B285" t="s">
-        <v>964</v>
+        <v>972</v>
       </c>
       <c r="C285" t="s">
-        <v>965</v>
+        <v>973</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -13881,7 +13929,7 @@
         <v>0.99999088788453128</v>
       </c>
       <c r="G285" t="s">
-        <v>966</v>
+        <v>974</v>
       </c>
       <c r="H285">
         <v>1</v>
@@ -13898,13 +13946,13 @@
     </row>
     <row r="286" spans="1:11">
       <c r="A286" t="s">
-        <v>967</v>
+        <v>975</v>
       </c>
       <c r="B286" t="s">
-        <v>968</v>
+        <v>976</v>
       </c>
       <c r="C286" t="s">
-        <v>969</v>
+        <v>977</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -13916,7 +13964,7 @@
         <v>0.40546209674036149</v>
       </c>
       <c r="G286" t="s">
-        <v>970</v>
+        <v>978</v>
       </c>
       <c r="H286">
         <v>0.21</v>
@@ -13925,7 +13973,7 @@
         <v>0.58109999999999995</v>
       </c>
       <c r="J286" t="s">
-        <v>971</v>
+        <v>979</v>
       </c>
       <c r="K286">
         <v>0</v>
@@ -13933,13 +13981,13 @@
     </row>
     <row r="287" spans="1:11">
       <c r="A287" t="s">
-        <v>972</v>
+        <v>980</v>
       </c>
       <c r="B287" t="s">
-        <v>973</v>
+        <v>981</v>
       </c>
       <c r="C287" t="s">
-        <v>973</v>
+        <v>981</v>
       </c>
       <c r="D287">
         <v>1</v>
@@ -13968,13 +14016,13 @@
     </row>
     <row r="288" spans="1:11">
       <c r="A288" t="s">
-        <v>974</v>
+        <v>982</v>
       </c>
       <c r="B288" t="s">
-        <v>975</v>
+        <v>983</v>
       </c>
       <c r="C288" t="s">
-        <v>975</v>
+        <v>983</v>
       </c>
       <c r="D288">
         <v>1</v>
@@ -14003,13 +14051,13 @@
     </row>
     <row r="289" spans="1:11">
       <c r="A289" t="s">
-        <v>976</v>
+        <v>984</v>
       </c>
       <c r="B289" t="s">
-        <v>977</v>
+        <v>985</v>
       </c>
       <c r="C289" t="s">
-        <v>978</v>
+        <v>986</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -14021,7 +14069,7 @@
         <v>0.99999451303155007</v>
       </c>
       <c r="G289" t="s">
-        <v>979</v>
+        <v>987</v>
       </c>
       <c r="H289">
         <v>0.92</v>
@@ -14030,7 +14078,7 @@
         <v>0.98659999999999992</v>
       </c>
       <c r="J289" t="s">
-        <v>980</v>
+        <v>988</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -14038,13 +14086,13 @@
     </row>
     <row r="290" spans="1:11">
       <c r="A290" t="s">
-        <v>981</v>
+        <v>989</v>
       </c>
       <c r="B290" t="s">
-        <v>982</v>
+        <v>990</v>
       </c>
       <c r="C290" t="s">
-        <v>982</v>
+        <v>990</v>
       </c>
       <c r="D290">
         <v>1</v>
@@ -14073,13 +14121,13 @@
     </row>
     <row r="291" spans="1:11">
       <c r="A291" t="s">
-        <v>983</v>
+        <v>991</v>
       </c>
       <c r="B291" t="s">
-        <v>984</v>
+        <v>992</v>
       </c>
       <c r="C291" t="s">
-        <v>984</v>
+        <v>992</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -14108,13 +14156,13 @@
     </row>
     <row r="292" spans="1:11">
       <c r="A292" t="s">
-        <v>985</v>
+        <v>993</v>
       </c>
       <c r="B292" t="s">
-        <v>986</v>
+        <v>994</v>
       </c>
       <c r="C292" t="s">
-        <v>987</v>
+        <v>995</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -14126,7 +14174,7 @@
         <v>0.93487490844375576</v>
       </c>
       <c r="G292" t="s">
-        <v>988</v>
+        <v>996</v>
       </c>
       <c r="H292">
         <v>0.9</v>
@@ -14135,7 +14183,7 @@
         <v>0.9909</v>
       </c>
       <c r="J292" t="s">
-        <v>989</v>
+        <v>997</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -14143,13 +14191,13 @@
     </row>
     <row r="293" spans="1:11">
       <c r="A293" t="s">
-        <v>990</v>
+        <v>998</v>
       </c>
       <c r="B293" t="s">
-        <v>991</v>
+        <v>999</v>
       </c>
       <c r="C293" t="s">
-        <v>991</v>
+        <v>999</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -14178,13 +14226,13 @@
     </row>
     <row r="294" spans="1:11">
       <c r="A294" t="s">
-        <v>992</v>
+        <v>1000</v>
       </c>
       <c r="B294" t="s">
-        <v>993</v>
+        <v>1001</v>
       </c>
       <c r="C294" t="s">
-        <v>994</v>
+        <v>1002</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -14196,7 +14244,7 @@
         <v>0.70304985209989224</v>
       </c>
       <c r="G294" t="s">
-        <v>995</v>
+        <v>1003</v>
       </c>
       <c r="H294">
         <v>0.66</v>
@@ -14205,7 +14253,7 @@
         <v>0.97909999999999997</v>
       </c>
       <c r="J294" t="s">
-        <v>996</v>
+        <v>1004</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -14213,13 +14261,13 @@
     </row>
     <row r="295" spans="1:11">
       <c r="A295" t="s">
-        <v>997</v>
+        <v>1005</v>
       </c>
       <c r="B295" t="s">
-        <v>998</v>
+        <v>1006</v>
       </c>
       <c r="C295" t="s">
-        <v>999</v>
+        <v>1007</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -14231,7 +14279,7 @@
         <v>0.99999902343750002</v>
       </c>
       <c r="G295" t="s">
-        <v>1000</v>
+        <v>1008</v>
       </c>
       <c r="H295">
         <v>1</v>
@@ -14240,7 +14288,7 @@
         <v>1</v>
       </c>
       <c r="J295" t="s">
-        <v>1001</v>
+        <v>1009</v>
       </c>
       <c r="K295">
         <v>0</v>
@@ -14248,13 +14296,13 @@
     </row>
     <row r="296" spans="1:11">
       <c r="A296" t="s">
-        <v>1002</v>
+        <v>1010</v>
       </c>
       <c r="B296" t="s">
-        <v>1003</v>
+        <v>1011</v>
       </c>
       <c r="C296" t="s">
-        <v>1004</v>
+        <v>1012</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -14266,7 +14314,7 @@
         <v>0.99999518411142041</v>
       </c>
       <c r="G296" t="s">
-        <v>1005</v>
+        <v>1013</v>
       </c>
       <c r="H296">
         <v>1</v>
@@ -14275,7 +14323,7 @@
         <v>1</v>
       </c>
       <c r="J296" t="s">
-        <v>1006</v>
+        <v>1014</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -14283,13 +14331,13 @@
     </row>
     <row r="297" spans="1:11">
       <c r="A297" t="s">
-        <v>1007</v>
+        <v>1015</v>
       </c>
       <c r="B297" t="s">
-        <v>1008</v>
+        <v>1016</v>
       </c>
       <c r="C297" t="s">
-        <v>1008</v>
+        <v>1016</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -14318,13 +14366,13 @@
     </row>
     <row r="298" spans="1:11">
       <c r="A298" t="s">
-        <v>1009</v>
+        <v>1017</v>
       </c>
       <c r="B298" t="s">
-        <v>1010</v>
+        <v>1018</v>
       </c>
       <c r="C298" t="s">
-        <v>1011</v>
+        <v>1019</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -14336,7 +14384,7 @@
         <v>0.96253492767915849</v>
       </c>
       <c r="G298" t="s">
-        <v>1012</v>
+        <v>1020</v>
       </c>
       <c r="H298">
         <v>0.83</v>
@@ -14345,7 +14393,7 @@
         <v>0.9484999999999999</v>
       </c>
       <c r="J298" t="s">
-        <v>1013</v>
+        <v>1021</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -14353,13 +14401,13 @@
     </row>
     <row r="299" spans="1:11">
       <c r="A299" t="s">
-        <v>1014</v>
+        <v>1022</v>
       </c>
       <c r="B299" t="s">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="C299" t="s">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -14388,13 +14436,13 @@
     </row>
     <row r="300" spans="1:11">
       <c r="A300" t="s">
-        <v>1016</v>
+        <v>1024</v>
       </c>
       <c r="B300" t="s">
-        <v>1017</v>
+        <v>1025</v>
       </c>
       <c r="C300" t="s">
-        <v>1018</v>
+        <v>1026</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -14406,7 +14454,7 @@
         <v>0.96831509702158602</v>
       </c>
       <c r="G300" t="s">
-        <v>1019</v>
+        <v>1027</v>
       </c>
       <c r="H300">
         <v>0.69</v>
@@ -14415,7 +14463,7 @@
         <v>0.87959999999999994</v>
       </c>
       <c r="J300" t="s">
-        <v>989</v>
+        <v>997</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -14423,13 +14471,13 @@
     </row>
     <row r="301" spans="1:11">
       <c r="A301" t="s">
-        <v>1020</v>
+        <v>1028</v>
       </c>
       <c r="B301" t="s">
-        <v>1021</v>
+        <v>1029</v>
       </c>
       <c r="C301" t="s">
-        <v>1021</v>
+        <v>1029</v>
       </c>
       <c r="D301">
         <v>1</v>
@@ -14458,13 +14506,13 @@
     </row>
     <row r="302" spans="1:11">
       <c r="A302" t="s">
-        <v>1022</v>
+        <v>1030</v>
       </c>
       <c r="B302" t="s">
-        <v>1023</v>
+        <v>1031</v>
       </c>
       <c r="C302" t="s">
-        <v>1024</v>
+        <v>1032</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -14476,7 +14524,7 @@
         <v>0.999996</v>
       </c>
       <c r="G302" t="s">
-        <v>1025</v>
+        <v>1033</v>
       </c>
       <c r="H302">
         <v>1</v>
@@ -14485,7 +14533,7 @@
         <v>1</v>
       </c>
       <c r="J302" t="s">
-        <v>1026</v>
+        <v>1034</v>
       </c>
       <c r="K302">
         <v>0</v>
@@ -14493,13 +14541,13 @@
     </row>
     <row r="303" spans="1:11">
       <c r="A303" t="s">
-        <v>1027</v>
+        <v>1035</v>
       </c>
       <c r="B303" t="s">
-        <v>1028</v>
+        <v>1036</v>
       </c>
       <c r="C303" t="s">
-        <v>1029</v>
+        <v>1037</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -14511,7 +14559,7 @@
         <v>0.74476011756102278</v>
       </c>
       <c r="G303" t="s">
-        <v>1030</v>
+        <v>1038</v>
       </c>
       <c r="H303">
         <v>0.56000000000000005</v>
@@ -14520,7 +14568,7 @@
         <v>0.76290000000000002</v>
       </c>
       <c r="J303" t="s">
-        <v>1031</v>
+        <v>1039</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -14528,13 +14576,13 @@
     </row>
     <row r="304" spans="1:11">
       <c r="A304" t="s">
-        <v>1032</v>
+        <v>1040</v>
       </c>
       <c r="B304" t="s">
-        <v>1033</v>
+        <v>1041</v>
       </c>
       <c r="C304" t="s">
-        <v>1034</v>
+        <v>1042</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -14546,7 +14594,7 @@
         <v>0.64379423183166962</v>
       </c>
       <c r="G304" t="s">
-        <v>1035</v>
+        <v>1043</v>
       </c>
       <c r="H304">
         <v>0.56999999999999995</v>
@@ -14555,7 +14603,7 @@
         <v>0.93209999999999993</v>
       </c>
       <c r="J304" t="s">
-        <v>1036</v>
+        <v>1044</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -14563,13 +14611,13 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305" t="s">
-        <v>1037</v>
+        <v>1045</v>
       </c>
       <c r="B305" t="s">
-        <v>1038</v>
+        <v>1046</v>
       </c>
       <c r="C305" t="s">
-        <v>1038</v>
+        <v>1046</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -14598,13 +14646,13 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306" t="s">
-        <v>1039</v>
+        <v>1047</v>
       </c>
       <c r="B306" t="s">
-        <v>1040</v>
+        <v>1048</v>
       </c>
       <c r="C306" t="s">
-        <v>1041</v>
+        <v>1049</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -14616,7 +14664,7 @@
         <v>0.97417177571210234</v>
       </c>
       <c r="G306" t="s">
-        <v>1042</v>
+        <v>1050</v>
       </c>
       <c r="H306">
         <v>0.93</v>
@@ -14625,7 +14673,7 @@
         <v>0.98209999999999997</v>
       </c>
       <c r="J306" t="s">
-        <v>1043</v>
+        <v>1051</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -14633,13 +14681,13 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307" t="s">
-        <v>1044</v>
+        <v>1052</v>
       </c>
       <c r="B307" t="s">
-        <v>1045</v>
+        <v>1053</v>
       </c>
       <c r="C307" t="s">
-        <v>1045</v>
+        <v>1053</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -14668,13 +14716,13 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308" t="s">
-        <v>1046</v>
+        <v>1054</v>
       </c>
       <c r="B308" t="s">
-        <v>1047</v>
+        <v>1055</v>
       </c>
       <c r="C308" t="s">
-        <v>1048</v>
+        <v>1056</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -14686,7 +14734,7 @@
         <v>0.98664022774046589</v>
       </c>
       <c r="G308" t="s">
-        <v>1049</v>
+        <v>1057</v>
       </c>
       <c r="H308">
         <v>0.97</v>
@@ -14695,7 +14743,7 @@
         <v>0.98909999999999998</v>
       </c>
       <c r="J308" t="s">
-        <v>1050</v>
+        <v>1058</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -14703,13 +14751,13 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309" t="s">
-        <v>1051</v>
+        <v>1059</v>
       </c>
       <c r="B309" t="s">
-        <v>1052</v>
+        <v>1060</v>
       </c>
       <c r="C309" t="s">
-        <v>1053</v>
+        <v>1061</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -14721,7 +14769,7 @@
         <v>0.99995890523547304</v>
       </c>
       <c r="G309" t="s">
-        <v>1054</v>
+        <v>1062</v>
       </c>
       <c r="H309">
         <v>1</v>
@@ -14730,7 +14778,7 @@
         <v>1</v>
       </c>
       <c r="J309" t="s">
-        <v>947</v>
+        <v>955</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -14738,13 +14786,13 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310" t="s">
-        <v>1055</v>
+        <v>1063</v>
       </c>
       <c r="B310" t="s">
-        <v>1056</v>
+        <v>1064</v>
       </c>
       <c r="C310" t="s">
-        <v>1056</v>
+        <v>1064</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -14773,13 +14821,13 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311" t="s">
-        <v>1057</v>
+        <v>1065</v>
       </c>
       <c r="B311" t="s">
-        <v>1058</v>
+        <v>1066</v>
       </c>
       <c r="C311" t="s">
-        <v>1059</v>
+        <v>1067</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -14791,7 +14839,7 @@
         <v>0.99998928326474623</v>
       </c>
       <c r="G311" t="s">
-        <v>1060</v>
+        <v>1068</v>
       </c>
       <c r="H311">
         <v>1</v>
@@ -14808,13 +14856,13 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312" t="s">
-        <v>1061</v>
+        <v>1069</v>
       </c>
       <c r="B312" t="s">
-        <v>1062</v>
+        <v>1070</v>
       </c>
       <c r="C312" t="s">
-        <v>1063</v>
+        <v>1071</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -14826,7 +14874,7 @@
         <v>0.97341886358453711</v>
       </c>
       <c r="G312" t="s">
-        <v>1064</v>
+        <v>1072</v>
       </c>
       <c r="H312">
         <v>0.94</v>
@@ -14835,7 +14883,7 @@
         <v>0.97719999999999996</v>
       </c>
       <c r="J312" t="s">
-        <v>1065</v>
+        <v>1073</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -14843,13 +14891,13 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313" t="s">
-        <v>1066</v>
+        <v>1074</v>
       </c>
       <c r="B313" t="s">
-        <v>1067</v>
+        <v>1075</v>
       </c>
       <c r="C313" t="s">
-        <v>1068</v>
+        <v>1076</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -14861,7 +14909,7 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313" t="s">
-        <v>1069</v>
+        <v>1077</v>
       </c>
       <c r="H313">
         <v>0.89</v>
@@ -14870,7 +14918,7 @@
         <v>0.9756999999999999</v>
       </c>
       <c r="J313" t="s">
-        <v>1070</v>
+        <v>1078</v>
       </c>
       <c r="K313">
         <v>0</v>
@@ -14878,13 +14926,13 @@
     </row>
     <row r="314" spans="1:11">
       <c r="A314" t="s">
-        <v>1071</v>
+        <v>1079</v>
       </c>
       <c r="B314" t="s">
-        <v>1072</v>
+        <v>1080</v>
       </c>
       <c r="C314" t="s">
-        <v>1073</v>
+        <v>1081</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -14896,7 +14944,7 @@
         <v>0.75858170895276666</v>
       </c>
       <c r="G314" t="s">
-        <v>1074</v>
+        <v>1082</v>
       </c>
       <c r="H314">
         <v>0.54</v>
@@ -14905,7 +14953,7 @@
         <v>0.68030000000000002</v>
       </c>
       <c r="J314" t="s">
-        <v>1075</v>
+        <v>1083</v>
       </c>
       <c r="K314">
         <v>0</v>
@@ -14913,13 +14961,13 @@
     </row>
     <row r="315" spans="1:11">
       <c r="A315" t="s">
-        <v>1076</v>
+        <v>1084</v>
       </c>
       <c r="B315" t="s">
-        <v>1077</v>
+        <v>1085</v>
       </c>
       <c r="C315" t="s">
-        <v>1078</v>
+        <v>1086</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -14931,7 +14979,7 @@
         <v>0.998317618783509</v>
       </c>
       <c r="G315" t="s">
-        <v>1079</v>
+        <v>1087</v>
       </c>
       <c r="H315">
         <v>0.9</v>
@@ -14940,7 +14988,7 @@
         <v>0.97470000000000001</v>
       </c>
       <c r="J315" t="s">
-        <v>1080</v>
+        <v>1088</v>
       </c>
       <c r="K315">
         <v>0</v>
@@ -14948,13 +14996,13 @@
     </row>
     <row r="316" spans="1:11">
       <c r="A316" t="s">
-        <v>1081</v>
+        <v>1089</v>
       </c>
       <c r="B316" t="s">
-        <v>1082</v>
+        <v>1090</v>
       </c>
       <c r="C316" t="s">
-        <v>1083</v>
+        <v>1091</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -14966,7 +15014,7 @@
         <v>0.95598287878305699</v>
       </c>
       <c r="G316" t="s">
-        <v>1084</v>
+        <v>1092</v>
       </c>
       <c r="H316">
         <v>0.92</v>
@@ -14975,7 +15023,7 @@
         <v>0.97089999999999999</v>
       </c>
       <c r="J316" t="s">
-        <v>1085</v>
+        <v>1093</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -14983,13 +15031,13 @@
     </row>
     <row r="317" spans="1:11">
       <c r="A317" t="s">
-        <v>1086</v>
+        <v>1094</v>
       </c>
       <c r="B317" t="s">
-        <v>1087</v>
+        <v>1095</v>
       </c>
       <c r="C317" t="s">
-        <v>1087</v>
+        <v>1095</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -15018,13 +15066,13 @@
     </row>
     <row r="318" spans="1:11">
       <c r="A318" t="s">
-        <v>1088</v>
+        <v>1096</v>
       </c>
       <c r="B318" t="s">
-        <v>1089</v>
+        <v>1097</v>
       </c>
       <c r="C318" t="s">
-        <v>1090</v>
+        <v>1098</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -15036,7 +15084,7 @@
         <v>0.95178740438847254</v>
       </c>
       <c r="G318" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="H318">
         <v>0.9</v>
@@ -15045,7 +15093,7 @@
         <v>0.97430000000000005</v>
       </c>
       <c r="J318" t="s">
-        <v>1092</v>
+        <v>1100</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -15053,13 +15101,13 @@
     </row>
     <row r="319" spans="1:11">
       <c r="A319" t="s">
-        <v>1093</v>
+        <v>1101</v>
       </c>
       <c r="B319" t="s">
-        <v>1094</v>
+        <v>1102</v>
       </c>
       <c r="C319" t="s">
-        <v>1095</v>
+        <v>1103</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -15071,7 +15119,7 @@
         <v>0.70336391437308876</v>
       </c>
       <c r="G319" t="s">
-        <v>1096</v>
+        <v>1104</v>
       </c>
       <c r="H319">
         <v>0.41</v>
@@ -15080,7 +15128,7 @@
         <v>0.80920000000000003</v>
       </c>
       <c r="J319" t="s">
-        <v>1097</v>
+        <v>1105</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -15088,13 +15136,13 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320" t="s">
-        <v>1098</v>
+        <v>1106</v>
       </c>
       <c r="B320" t="s">
-        <v>1099</v>
+        <v>1107</v>
       </c>
       <c r="C320" t="s">
-        <v>1099</v>
+        <v>1107</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -15123,13 +15171,13 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1100</v>
+        <v>1108</v>
       </c>
       <c r="B321" t="s">
-        <v>1101</v>
+        <v>1109</v>
       </c>
       <c r="C321" t="s">
-        <v>1102</v>
+        <v>1110</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -15141,7 +15189,7 @@
         <v>0.99849640734645617</v>
       </c>
       <c r="G321" t="s">
-        <v>1103</v>
+        <v>1111</v>
       </c>
       <c r="H321">
         <v>0.98</v>
@@ -15150,7 +15198,7 @@
         <v>0.99470000000000003</v>
       </c>
       <c r="J321" t="s">
-        <v>1104</v>
+        <v>1112</v>
       </c>
       <c r="K321">
         <v>0</v>
@@ -15158,13 +15206,13 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1105</v>
+        <v>1113</v>
       </c>
       <c r="B322" t="s">
-        <v>1106</v>
+        <v>1114</v>
       </c>
       <c r="C322" t="s">
-        <v>1106</v>
+        <v>1114</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -15193,13 +15241,13 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1107</v>
+        <v>1115</v>
       </c>
       <c r="B323" t="s">
-        <v>1108</v>
+        <v>1116</v>
       </c>
       <c r="C323" t="s">
-        <v>1108</v>
+        <v>1116</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -15228,13 +15276,13 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1109</v>
+        <v>1117</v>
       </c>
       <c r="B324" t="s">
-        <v>1110</v>
+        <v>1118</v>
       </c>
       <c r="C324" t="s">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -15246,7 +15294,7 @@
         <v>0.99690437876548454</v>
       </c>
       <c r="G324" t="s">
-        <v>1112</v>
+        <v>1120</v>
       </c>
       <c r="H324">
         <v>0.95</v>
@@ -15255,7 +15303,7 @@
         <v>0.98730000000000007</v>
       </c>
       <c r="J324" t="s">
-        <v>1113</v>
+        <v>1121</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -15263,13 +15311,13 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1114</v>
+        <v>1122</v>
       </c>
       <c r="B325" t="s">
-        <v>1115</v>
+        <v>1123</v>
       </c>
       <c r="C325" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -15281,7 +15329,7 @@
         <v>0.9999968246710359</v>
       </c>
       <c r="G325" t="s">
-        <v>1117</v>
+        <v>1125</v>
       </c>
       <c r="H325">
         <v>1</v>
@@ -15290,7 +15338,7 @@
         <v>1</v>
       </c>
       <c r="J325" t="s">
-        <v>1118</v>
+        <v>1126</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -15298,13 +15346,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1119</v>
+        <v>1127</v>
       </c>
       <c r="B326" t="s">
-        <v>1120</v>
+        <v>1128</v>
       </c>
       <c r="C326" t="s">
-        <v>1120</v>
+        <v>1128</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -15333,13 +15381,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1121</v>
+        <v>1129</v>
       </c>
       <c r="B327" t="s">
-        <v>1122</v>
+        <v>1130</v>
       </c>
       <c r="C327" t="s">
-        <v>1122</v>
+        <v>1130</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Aggiunte nuove analisi CodeT5_770
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/Analisi_CodeT5_770.xlsx
+++ b/HE/W_in_progress/Analisi_CodeT5_770.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28317"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28AAE9D6-7468-456B-BAC8-51747266CC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E67A25F-FE1D-4852-9A73-40C83D12C9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="1140">
   <si>
     <t>IN</t>
   </si>
@@ -2736,6 +2736,9 @@
     <t>0.71999999516928</t>
   </si>
   <si>
+    <t>Non fa una conversione BCD</t>
+  </si>
+  <si>
     <t>Create a basic frequency meter</t>
   </si>
   <si>
@@ -2751,6 +2754,9 @@
     <t>0.6666666619654322</t>
   </si>
   <si>
+    <t>Non genera un frequenzimetro</t>
+  </si>
+  <si>
     <t>Write a digital differentiator of N-bit with the signals clk and input_data (N-bit) as input and the signal differentiated_data (N-bit) as output.</t>
   </si>
   <si>
@@ -2766,6 +2772,9 @@
     <t>0.851063824796288</t>
   </si>
   <si>
+    <t>Non fa la differenziazione</t>
+  </si>
+  <si>
     <t>Define a digital integrator of N-bit with the signals clock, reset, and data_in (N-bit) as input and the signal integrated_output (N-bit) as output.</t>
   </si>
   <si>
@@ -2781,6 +2790,9 @@
     <t>0.7678571378635205</t>
   </si>
   <si>
+    <t>Non è un integratore</t>
+  </si>
+  <si>
     <t>Define a CRC generator of N-bit with the signals data_in (N-bit) and polynomial (M-bit) as input and the signal CRC_value (M-bit) as output.</t>
   </si>
   <si>
@@ -2796,6 +2808,9 @@
     <t>0.5901639294316046</t>
   </si>
   <si>
+    <t>Va bene</t>
+  </si>
+  <si>
     <t>Generate a priority encoder of 2^M-to-M with the signal requests (2^M-bit) as input and the signals encoded (M-bit) and valid as output.</t>
   </si>
   <si>
@@ -2811,6 +2826,9 @@
     <t>0.6949152492387246</t>
   </si>
   <si>
+    <t>Non proprio un encoder</t>
+  </si>
+  <si>
     <t>Define an unsigned divider of N-bit with the signals dividend (N-bit) and divisor (N-bit) as input and the signals quotient (N-bit) and remainder (N-bit) as output.</t>
   </si>
   <si>
@@ -2826,6 +2844,9 @@
     <t>0.5090909041504134</t>
   </si>
   <si>
+    <t>Ci sta</t>
+  </si>
+  <si>
     <t>Implement a basic I2C master controller</t>
   </si>
   <si>
@@ -2838,6 +2859,9 @@
     <t>0.35294117220155713</t>
   </si>
   <si>
+    <t xml:space="preserve">Proprio n'alrtra cosa </t>
+  </si>
+  <si>
     <t>Create a basic DDS (Direct Digital Synthesis) waveform generator</t>
   </si>
   <si>
@@ -2851,6 +2875,9 @@
   </si>
   <si>
     <t>0.4193548338969824</t>
+  </si>
+  <si>
+    <t>E' un DSS (anche se è un po strano)</t>
   </si>
   <si>
     <t>Write a comparator circuit of K-bit with the signals value1 (K-bit) and value2 (K-bit) as input and the signals greater, equal, and smaller as output.</t>
@@ -3796,8 +3823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C244" workbookViewId="0">
-      <selection activeCell="L266" sqref="L266"/>
+    <sheetView tabSelected="1" topLeftCell="B256" workbookViewId="0">
+      <selection activeCell="L276" sqref="L276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13276,7 +13303,7 @@
         <v>895</v>
       </c>
       <c r="K266">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267" spans="1:12">
@@ -13313,16 +13340,19 @@
       <c r="K267">
         <v>0</v>
       </c>
+      <c r="L267" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="268" spans="1:12">
       <c r="A268" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B268" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C268" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -13334,7 +13364,7 @@
         <v>0.42987585923874011</v>
       </c>
       <c r="G268" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="H268">
         <v>0</v>
@@ -13343,21 +13373,24 @@
         <v>0.9335</v>
       </c>
       <c r="J268" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="K268">
         <v>0</v>
+      </c>
+      <c r="L268" t="s">
+        <v>907</v>
       </c>
     </row>
     <row r="269" spans="1:12">
       <c r="A269" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B269" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C269" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -13369,7 +13402,7 @@
         <v>0.86196594368483526</v>
       </c>
       <c r="G269" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="H269">
         <v>0.76</v>
@@ -13378,21 +13411,24 @@
         <v>0.94590000000000007</v>
       </c>
       <c r="J269" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="K269">
         <v>0</v>
+      </c>
+      <c r="L269" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="270" spans="1:12">
       <c r="A270" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="B270" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="C270" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -13404,7 +13440,7 @@
         <v>0.88802454698719147</v>
       </c>
       <c r="G270" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="H270">
         <v>0.73</v>
@@ -13413,21 +13449,24 @@
         <v>0.97549999999999992</v>
       </c>
       <c r="J270" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="K270">
         <v>0</v>
+      </c>
+      <c r="L270" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="271" spans="1:12">
       <c r="A271" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c r="B271" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="C271" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -13439,7 +13478,7 @@
         <v>0.58879799469651517</v>
       </c>
       <c r="G271" t="s">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c r="H271">
         <v>0.16</v>
@@ -13448,21 +13487,24 @@
         <v>0.85709999999999997</v>
       </c>
       <c r="J271" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="K271">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L271" t="s">
+        <v>925</v>
       </c>
     </row>
     <row r="272" spans="1:12">
       <c r="A272" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="B272" t="s">
-        <v>922</v>
+        <v>927</v>
       </c>
       <c r="C272" t="s">
-        <v>923</v>
+        <v>928</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -13474,7 +13516,7 @@
         <v>0.66424709652589042</v>
       </c>
       <c r="G272" t="s">
-        <v>924</v>
+        <v>929</v>
       </c>
       <c r="H272">
         <v>0</v>
@@ -13483,21 +13525,24 @@
         <v>0.77150000000000007</v>
       </c>
       <c r="J272" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="K272">
         <v>0</v>
       </c>
-    </row>
-    <row r="273" spans="1:11">
+      <c r="L272" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12">
       <c r="A273" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="B273" t="s">
-        <v>927</v>
+        <v>933</v>
       </c>
       <c r="C273" t="s">
-        <v>928</v>
+        <v>934</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -13509,7 +13554,7 @@
         <v>0.52442395360121852</v>
       </c>
       <c r="G273" t="s">
-        <v>929</v>
+        <v>935</v>
       </c>
       <c r="H273">
         <v>0</v>
@@ -13518,18 +13563,21 @@
         <v>0.73470000000000002</v>
       </c>
       <c r="J273" t="s">
-        <v>930</v>
+        <v>936</v>
       </c>
       <c r="K273">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L273" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12">
       <c r="A274" t="s">
-        <v>931</v>
+        <v>938</v>
       </c>
       <c r="B274" t="s">
-        <v>932</v>
+        <v>939</v>
       </c>
       <c r="C274" t="s">
         <v>887</v>
@@ -13544,7 +13592,7 @@
         <v>0.17054273168875969</v>
       </c>
       <c r="G274" t="s">
-        <v>933</v>
+        <v>940</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -13553,21 +13601,24 @@
         <v>0.67669999999999997</v>
       </c>
       <c r="J274" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="K274">
         <v>0</v>
       </c>
-    </row>
-    <row r="275" spans="1:11">
+      <c r="L274" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12">
       <c r="A275" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="B275" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="C275" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -13579,7 +13630,7 @@
         <v>0.25958012686025911</v>
       </c>
       <c r="G275" t="s">
-        <v>938</v>
+        <v>946</v>
       </c>
       <c r="H275">
         <v>0</v>
@@ -13588,21 +13639,24 @@
         <v>0.79760000000000009</v>
       </c>
       <c r="J275" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="K275">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L275" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12">
       <c r="A276" t="s">
-        <v>940</v>
+        <v>949</v>
       </c>
       <c r="B276" t="s">
-        <v>941</v>
+        <v>950</v>
       </c>
       <c r="C276" t="s">
-        <v>942</v>
+        <v>951</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -13614,7 +13668,7 @@
         <v>0.48741343083544247</v>
       </c>
       <c r="G276" t="s">
-        <v>943</v>
+        <v>952</v>
       </c>
       <c r="H276">
         <v>0.52</v>
@@ -13623,21 +13677,21 @@
         <v>0.80959999999999999</v>
       </c>
       <c r="J276" t="s">
-        <v>944</v>
+        <v>953</v>
       </c>
       <c r="K276">
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:11">
+    <row r="277" spans="1:12">
       <c r="A277" t="s">
-        <v>945</v>
+        <v>954</v>
       </c>
       <c r="B277" t="s">
-        <v>946</v>
+        <v>955</v>
       </c>
       <c r="C277" t="s">
-        <v>947</v>
+        <v>956</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -13649,7 +13703,7 @@
         <v>0.89602265394280345</v>
       </c>
       <c r="G277" t="s">
-        <v>948</v>
+        <v>957</v>
       </c>
       <c r="H277">
         <v>0.77</v>
@@ -13664,15 +13718,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:11">
+    <row r="278" spans="1:12">
       <c r="A278" t="s">
-        <v>949</v>
+        <v>958</v>
       </c>
       <c r="B278" t="s">
-        <v>950</v>
+        <v>959</v>
       </c>
       <c r="C278" t="s">
-        <v>950</v>
+        <v>959</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -13699,15 +13753,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:11">
+    <row r="279" spans="1:12">
       <c r="A279" t="s">
-        <v>951</v>
+        <v>960</v>
       </c>
       <c r="B279" t="s">
-        <v>952</v>
+        <v>961</v>
       </c>
       <c r="C279" t="s">
-        <v>953</v>
+        <v>962</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -13719,7 +13773,7 @@
         <v>0.99997459736828731</v>
       </c>
       <c r="G279" t="s">
-        <v>954</v>
+        <v>963</v>
       </c>
       <c r="H279">
         <v>1</v>
@@ -13728,21 +13782,21 @@
         <v>1</v>
       </c>
       <c r="J279" t="s">
-        <v>955</v>
+        <v>964</v>
       </c>
       <c r="K279">
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:11">
+    <row r="280" spans="1:12">
       <c r="A280" t="s">
-        <v>956</v>
+        <v>965</v>
       </c>
       <c r="B280" t="s">
-        <v>957</v>
+        <v>966</v>
       </c>
       <c r="C280" t="s">
-        <v>957</v>
+        <v>966</v>
       </c>
       <c r="D280">
         <v>1</v>
@@ -13769,15 +13823,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:11">
+    <row r="281" spans="1:12">
       <c r="A281" t="s">
-        <v>958</v>
+        <v>967</v>
       </c>
       <c r="B281" t="s">
-        <v>959</v>
+        <v>968</v>
       </c>
       <c r="C281" t="s">
-        <v>959</v>
+        <v>968</v>
       </c>
       <c r="D281">
         <v>1</v>
@@ -13804,15 +13858,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:11">
+    <row r="282" spans="1:12">
       <c r="A282" t="s">
-        <v>960</v>
+        <v>969</v>
       </c>
       <c r="B282" t="s">
-        <v>961</v>
+        <v>970</v>
       </c>
       <c r="C282" t="s">
-        <v>961</v>
+        <v>970</v>
       </c>
       <c r="D282">
         <v>1</v>
@@ -13839,15 +13893,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:11">
+    <row r="283" spans="1:12">
       <c r="A283" t="s">
-        <v>962</v>
+        <v>971</v>
       </c>
       <c r="B283" t="s">
-        <v>963</v>
+        <v>972</v>
       </c>
       <c r="C283" t="s">
-        <v>964</v>
+        <v>973</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -13859,7 +13913,7 @@
         <v>0.16107144603648099</v>
       </c>
       <c r="G283" t="s">
-        <v>965</v>
+        <v>974</v>
       </c>
       <c r="H283">
         <v>0.15</v>
@@ -13868,21 +13922,21 @@
         <v>8.2400000000000001E-2</v>
       </c>
       <c r="J283" t="s">
-        <v>966</v>
+        <v>975</v>
       </c>
       <c r="K283">
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:11">
+    <row r="284" spans="1:12">
       <c r="A284" t="s">
-        <v>967</v>
+        <v>976</v>
       </c>
       <c r="B284" t="s">
-        <v>968</v>
+        <v>977</v>
       </c>
       <c r="C284" t="s">
-        <v>969</v>
+        <v>978</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -13894,7 +13948,7 @@
         <v>0.99985185185185188</v>
       </c>
       <c r="G284" t="s">
-        <v>970</v>
+        <v>979</v>
       </c>
       <c r="H284">
         <v>0.92</v>
@@ -13909,15 +13963,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:11">
+    <row r="285" spans="1:12">
       <c r="A285" t="s">
-        <v>971</v>
+        <v>980</v>
       </c>
       <c r="B285" t="s">
-        <v>972</v>
+        <v>981</v>
       </c>
       <c r="C285" t="s">
-        <v>973</v>
+        <v>982</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -13929,7 +13983,7 @@
         <v>0.99999088788453128</v>
       </c>
       <c r="G285" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="H285">
         <v>1</v>
@@ -13944,15 +13998,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:11">
+    <row r="286" spans="1:12">
       <c r="A286" t="s">
-        <v>975</v>
+        <v>984</v>
       </c>
       <c r="B286" t="s">
-        <v>976</v>
+        <v>985</v>
       </c>
       <c r="C286" t="s">
-        <v>977</v>
+        <v>986</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -13964,7 +14018,7 @@
         <v>0.40546209674036149</v>
       </c>
       <c r="G286" t="s">
-        <v>978</v>
+        <v>987</v>
       </c>
       <c r="H286">
         <v>0.21</v>
@@ -13973,21 +14027,21 @@
         <v>0.58109999999999995</v>
       </c>
       <c r="J286" t="s">
-        <v>979</v>
+        <v>988</v>
       </c>
       <c r="K286">
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:11">
+    <row r="287" spans="1:12">
       <c r="A287" t="s">
-        <v>980</v>
+        <v>989</v>
       </c>
       <c r="B287" t="s">
-        <v>981</v>
+        <v>990</v>
       </c>
       <c r="C287" t="s">
-        <v>981</v>
+        <v>990</v>
       </c>
       <c r="D287">
         <v>1</v>
@@ -14014,15 +14068,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:11">
+    <row r="288" spans="1:12">
       <c r="A288" t="s">
-        <v>982</v>
+        <v>991</v>
       </c>
       <c r="B288" t="s">
-        <v>983</v>
+        <v>992</v>
       </c>
       <c r="C288" t="s">
-        <v>983</v>
+        <v>992</v>
       </c>
       <c r="D288">
         <v>1</v>
@@ -14051,13 +14105,13 @@
     </row>
     <row r="289" spans="1:11">
       <c r="A289" t="s">
-        <v>984</v>
+        <v>993</v>
       </c>
       <c r="B289" t="s">
-        <v>985</v>
+        <v>994</v>
       </c>
       <c r="C289" t="s">
-        <v>986</v>
+        <v>995</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -14069,7 +14123,7 @@
         <v>0.99999451303155007</v>
       </c>
       <c r="G289" t="s">
-        <v>987</v>
+        <v>996</v>
       </c>
       <c r="H289">
         <v>0.92</v>
@@ -14078,7 +14132,7 @@
         <v>0.98659999999999992</v>
       </c>
       <c r="J289" t="s">
-        <v>988</v>
+        <v>997</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -14086,13 +14140,13 @@
     </row>
     <row r="290" spans="1:11">
       <c r="A290" t="s">
-        <v>989</v>
+        <v>998</v>
       </c>
       <c r="B290" t="s">
-        <v>990</v>
+        <v>999</v>
       </c>
       <c r="C290" t="s">
-        <v>990</v>
+        <v>999</v>
       </c>
       <c r="D290">
         <v>1</v>
@@ -14121,13 +14175,13 @@
     </row>
     <row r="291" spans="1:11">
       <c r="A291" t="s">
-        <v>991</v>
+        <v>1000</v>
       </c>
       <c r="B291" t="s">
-        <v>992</v>
+        <v>1001</v>
       </c>
       <c r="C291" t="s">
-        <v>992</v>
+        <v>1001</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -14156,13 +14210,13 @@
     </row>
     <row r="292" spans="1:11">
       <c r="A292" t="s">
-        <v>993</v>
+        <v>1002</v>
       </c>
       <c r="B292" t="s">
-        <v>994</v>
+        <v>1003</v>
       </c>
       <c r="C292" t="s">
-        <v>995</v>
+        <v>1004</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -14174,7 +14228,7 @@
         <v>0.93487490844375576</v>
       </c>
       <c r="G292" t="s">
-        <v>996</v>
+        <v>1005</v>
       </c>
       <c r="H292">
         <v>0.9</v>
@@ -14183,7 +14237,7 @@
         <v>0.9909</v>
       </c>
       <c r="J292" t="s">
-        <v>997</v>
+        <v>1006</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -14191,13 +14245,13 @@
     </row>
     <row r="293" spans="1:11">
       <c r="A293" t="s">
-        <v>998</v>
+        <v>1007</v>
       </c>
       <c r="B293" t="s">
-        <v>999</v>
+        <v>1008</v>
       </c>
       <c r="C293" t="s">
-        <v>999</v>
+        <v>1008</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -14226,13 +14280,13 @@
     </row>
     <row r="294" spans="1:11">
       <c r="A294" t="s">
-        <v>1000</v>
+        <v>1009</v>
       </c>
       <c r="B294" t="s">
-        <v>1001</v>
+        <v>1010</v>
       </c>
       <c r="C294" t="s">
-        <v>1002</v>
+        <v>1011</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -14244,7 +14298,7 @@
         <v>0.70304985209989224</v>
       </c>
       <c r="G294" t="s">
-        <v>1003</v>
+        <v>1012</v>
       </c>
       <c r="H294">
         <v>0.66</v>
@@ -14253,7 +14307,7 @@
         <v>0.97909999999999997</v>
       </c>
       <c r="J294" t="s">
-        <v>1004</v>
+        <v>1013</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -14261,13 +14315,13 @@
     </row>
     <row r="295" spans="1:11">
       <c r="A295" t="s">
-        <v>1005</v>
+        <v>1014</v>
       </c>
       <c r="B295" t="s">
-        <v>1006</v>
+        <v>1015</v>
       </c>
       <c r="C295" t="s">
-        <v>1007</v>
+        <v>1016</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -14279,7 +14333,7 @@
         <v>0.99999902343750002</v>
       </c>
       <c r="G295" t="s">
-        <v>1008</v>
+        <v>1017</v>
       </c>
       <c r="H295">
         <v>1</v>
@@ -14288,7 +14342,7 @@
         <v>1</v>
       </c>
       <c r="J295" t="s">
-        <v>1009</v>
+        <v>1018</v>
       </c>
       <c r="K295">
         <v>0</v>
@@ -14296,13 +14350,13 @@
     </row>
     <row r="296" spans="1:11">
       <c r="A296" t="s">
-        <v>1010</v>
+        <v>1019</v>
       </c>
       <c r="B296" t="s">
-        <v>1011</v>
+        <v>1020</v>
       </c>
       <c r="C296" t="s">
-        <v>1012</v>
+        <v>1021</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -14314,7 +14368,7 @@
         <v>0.99999518411142041</v>
       </c>
       <c r="G296" t="s">
-        <v>1013</v>
+        <v>1022</v>
       </c>
       <c r="H296">
         <v>1</v>
@@ -14323,7 +14377,7 @@
         <v>1</v>
       </c>
       <c r="J296" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -14331,13 +14385,13 @@
     </row>
     <row r="297" spans="1:11">
       <c r="A297" t="s">
-        <v>1015</v>
+        <v>1024</v>
       </c>
       <c r="B297" t="s">
-        <v>1016</v>
+        <v>1025</v>
       </c>
       <c r="C297" t="s">
-        <v>1016</v>
+        <v>1025</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -14366,13 +14420,13 @@
     </row>
     <row r="298" spans="1:11">
       <c r="A298" t="s">
-        <v>1017</v>
+        <v>1026</v>
       </c>
       <c r="B298" t="s">
-        <v>1018</v>
+        <v>1027</v>
       </c>
       <c r="C298" t="s">
-        <v>1019</v>
+        <v>1028</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -14384,7 +14438,7 @@
         <v>0.96253492767915849</v>
       </c>
       <c r="G298" t="s">
-        <v>1020</v>
+        <v>1029</v>
       </c>
       <c r="H298">
         <v>0.83</v>
@@ -14393,7 +14447,7 @@
         <v>0.9484999999999999</v>
       </c>
       <c r="J298" t="s">
-        <v>1021</v>
+        <v>1030</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -14401,13 +14455,13 @@
     </row>
     <row r="299" spans="1:11">
       <c r="A299" t="s">
-        <v>1022</v>
+        <v>1031</v>
       </c>
       <c r="B299" t="s">
-        <v>1023</v>
+        <v>1032</v>
       </c>
       <c r="C299" t="s">
-        <v>1023</v>
+        <v>1032</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -14436,13 +14490,13 @@
     </row>
     <row r="300" spans="1:11">
       <c r="A300" t="s">
-        <v>1024</v>
+        <v>1033</v>
       </c>
       <c r="B300" t="s">
-        <v>1025</v>
+        <v>1034</v>
       </c>
       <c r="C300" t="s">
-        <v>1026</v>
+        <v>1035</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -14454,7 +14508,7 @@
         <v>0.96831509702158602</v>
       </c>
       <c r="G300" t="s">
-        <v>1027</v>
+        <v>1036</v>
       </c>
       <c r="H300">
         <v>0.69</v>
@@ -14463,7 +14517,7 @@
         <v>0.87959999999999994</v>
       </c>
       <c r="J300" t="s">
-        <v>997</v>
+        <v>1006</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -14471,13 +14525,13 @@
     </row>
     <row r="301" spans="1:11">
       <c r="A301" t="s">
-        <v>1028</v>
+        <v>1037</v>
       </c>
       <c r="B301" t="s">
-        <v>1029</v>
+        <v>1038</v>
       </c>
       <c r="C301" t="s">
-        <v>1029</v>
+        <v>1038</v>
       </c>
       <c r="D301">
         <v>1</v>
@@ -14506,13 +14560,13 @@
     </row>
     <row r="302" spans="1:11">
       <c r="A302" t="s">
-        <v>1030</v>
+        <v>1039</v>
       </c>
       <c r="B302" t="s">
-        <v>1031</v>
+        <v>1040</v>
       </c>
       <c r="C302" t="s">
-        <v>1032</v>
+        <v>1041</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -14524,7 +14578,7 @@
         <v>0.999996</v>
       </c>
       <c r="G302" t="s">
-        <v>1033</v>
+        <v>1042</v>
       </c>
       <c r="H302">
         <v>1</v>
@@ -14533,7 +14587,7 @@
         <v>1</v>
       </c>
       <c r="J302" t="s">
-        <v>1034</v>
+        <v>1043</v>
       </c>
       <c r="K302">
         <v>0</v>
@@ -14541,13 +14595,13 @@
     </row>
     <row r="303" spans="1:11">
       <c r="A303" t="s">
-        <v>1035</v>
+        <v>1044</v>
       </c>
       <c r="B303" t="s">
-        <v>1036</v>
+        <v>1045</v>
       </c>
       <c r="C303" t="s">
-        <v>1037</v>
+        <v>1046</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -14559,7 +14613,7 @@
         <v>0.74476011756102278</v>
       </c>
       <c r="G303" t="s">
-        <v>1038</v>
+        <v>1047</v>
       </c>
       <c r="H303">
         <v>0.56000000000000005</v>
@@ -14568,7 +14622,7 @@
         <v>0.76290000000000002</v>
       </c>
       <c r="J303" t="s">
-        <v>1039</v>
+        <v>1048</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -14576,13 +14630,13 @@
     </row>
     <row r="304" spans="1:11">
       <c r="A304" t="s">
-        <v>1040</v>
+        <v>1049</v>
       </c>
       <c r="B304" t="s">
-        <v>1041</v>
+        <v>1050</v>
       </c>
       <c r="C304" t="s">
-        <v>1042</v>
+        <v>1051</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -14594,7 +14648,7 @@
         <v>0.64379423183166962</v>
       </c>
       <c r="G304" t="s">
-        <v>1043</v>
+        <v>1052</v>
       </c>
       <c r="H304">
         <v>0.56999999999999995</v>
@@ -14603,7 +14657,7 @@
         <v>0.93209999999999993</v>
       </c>
       <c r="J304" t="s">
-        <v>1044</v>
+        <v>1053</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -14611,13 +14665,13 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305" t="s">
-        <v>1045</v>
+        <v>1054</v>
       </c>
       <c r="B305" t="s">
-        <v>1046</v>
+        <v>1055</v>
       </c>
       <c r="C305" t="s">
-        <v>1046</v>
+        <v>1055</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -14646,13 +14700,13 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306" t="s">
-        <v>1047</v>
+        <v>1056</v>
       </c>
       <c r="B306" t="s">
-        <v>1048</v>
+        <v>1057</v>
       </c>
       <c r="C306" t="s">
-        <v>1049</v>
+        <v>1058</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -14664,7 +14718,7 @@
         <v>0.97417177571210234</v>
       </c>
       <c r="G306" t="s">
-        <v>1050</v>
+        <v>1059</v>
       </c>
       <c r="H306">
         <v>0.93</v>
@@ -14673,7 +14727,7 @@
         <v>0.98209999999999997</v>
       </c>
       <c r="J306" t="s">
-        <v>1051</v>
+        <v>1060</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -14681,13 +14735,13 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307" t="s">
-        <v>1052</v>
+        <v>1061</v>
       </c>
       <c r="B307" t="s">
-        <v>1053</v>
+        <v>1062</v>
       </c>
       <c r="C307" t="s">
-        <v>1053</v>
+        <v>1062</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -14716,13 +14770,13 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308" t="s">
-        <v>1054</v>
+        <v>1063</v>
       </c>
       <c r="B308" t="s">
-        <v>1055</v>
+        <v>1064</v>
       </c>
       <c r="C308" t="s">
-        <v>1056</v>
+        <v>1065</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -14734,7 +14788,7 @@
         <v>0.98664022774046589</v>
       </c>
       <c r="G308" t="s">
-        <v>1057</v>
+        <v>1066</v>
       </c>
       <c r="H308">
         <v>0.97</v>
@@ -14743,7 +14797,7 @@
         <v>0.98909999999999998</v>
       </c>
       <c r="J308" t="s">
-        <v>1058</v>
+        <v>1067</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -14751,13 +14805,13 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309" t="s">
-        <v>1059</v>
+        <v>1068</v>
       </c>
       <c r="B309" t="s">
-        <v>1060</v>
+        <v>1069</v>
       </c>
       <c r="C309" t="s">
-        <v>1061</v>
+        <v>1070</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -14769,7 +14823,7 @@
         <v>0.99995890523547304</v>
       </c>
       <c r="G309" t="s">
-        <v>1062</v>
+        <v>1071</v>
       </c>
       <c r="H309">
         <v>1</v>
@@ -14778,7 +14832,7 @@
         <v>1</v>
       </c>
       <c r="J309" t="s">
-        <v>955</v>
+        <v>964</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -14786,13 +14840,13 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310" t="s">
-        <v>1063</v>
+        <v>1072</v>
       </c>
       <c r="B310" t="s">
-        <v>1064</v>
+        <v>1073</v>
       </c>
       <c r="C310" t="s">
-        <v>1064</v>
+        <v>1073</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -14821,13 +14875,13 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311" t="s">
-        <v>1065</v>
+        <v>1074</v>
       </c>
       <c r="B311" t="s">
-        <v>1066</v>
+        <v>1075</v>
       </c>
       <c r="C311" t="s">
-        <v>1067</v>
+        <v>1076</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -14839,7 +14893,7 @@
         <v>0.99998928326474623</v>
       </c>
       <c r="G311" t="s">
-        <v>1068</v>
+        <v>1077</v>
       </c>
       <c r="H311">
         <v>1</v>
@@ -14856,13 +14910,13 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312" t="s">
-        <v>1069</v>
+        <v>1078</v>
       </c>
       <c r="B312" t="s">
-        <v>1070</v>
+        <v>1079</v>
       </c>
       <c r="C312" t="s">
-        <v>1071</v>
+        <v>1080</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -14874,7 +14928,7 @@
         <v>0.97341886358453711</v>
       </c>
       <c r="G312" t="s">
-        <v>1072</v>
+        <v>1081</v>
       </c>
       <c r="H312">
         <v>0.94</v>
@@ -14883,7 +14937,7 @@
         <v>0.97719999999999996</v>
       </c>
       <c r="J312" t="s">
-        <v>1073</v>
+        <v>1082</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -14891,13 +14945,13 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313" t="s">
-        <v>1074</v>
+        <v>1083</v>
       </c>
       <c r="B313" t="s">
-        <v>1075</v>
+        <v>1084</v>
       </c>
       <c r="C313" t="s">
-        <v>1076</v>
+        <v>1085</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -14909,7 +14963,7 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313" t="s">
-        <v>1077</v>
+        <v>1086</v>
       </c>
       <c r="H313">
         <v>0.89</v>
@@ -14918,7 +14972,7 @@
         <v>0.9756999999999999</v>
       </c>
       <c r="J313" t="s">
-        <v>1078</v>
+        <v>1087</v>
       </c>
       <c r="K313">
         <v>0</v>
@@ -14926,13 +14980,13 @@
     </row>
     <row r="314" spans="1:11">
       <c r="A314" t="s">
-        <v>1079</v>
+        <v>1088</v>
       </c>
       <c r="B314" t="s">
-        <v>1080</v>
+        <v>1089</v>
       </c>
       <c r="C314" t="s">
-        <v>1081</v>
+        <v>1090</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -14944,7 +14998,7 @@
         <v>0.75858170895276666</v>
       </c>
       <c r="G314" t="s">
-        <v>1082</v>
+        <v>1091</v>
       </c>
       <c r="H314">
         <v>0.54</v>
@@ -14953,7 +15007,7 @@
         <v>0.68030000000000002</v>
       </c>
       <c r="J314" t="s">
-        <v>1083</v>
+        <v>1092</v>
       </c>
       <c r="K314">
         <v>0</v>
@@ -14961,13 +15015,13 @@
     </row>
     <row r="315" spans="1:11">
       <c r="A315" t="s">
-        <v>1084</v>
+        <v>1093</v>
       </c>
       <c r="B315" t="s">
-        <v>1085</v>
+        <v>1094</v>
       </c>
       <c r="C315" t="s">
-        <v>1086</v>
+        <v>1095</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -14979,7 +15033,7 @@
         <v>0.998317618783509</v>
       </c>
       <c r="G315" t="s">
-        <v>1087</v>
+        <v>1096</v>
       </c>
       <c r="H315">
         <v>0.9</v>
@@ -14988,7 +15042,7 @@
         <v>0.97470000000000001</v>
       </c>
       <c r="J315" t="s">
-        <v>1088</v>
+        <v>1097</v>
       </c>
       <c r="K315">
         <v>0</v>
@@ -14996,13 +15050,13 @@
     </row>
     <row r="316" spans="1:11">
       <c r="A316" t="s">
-        <v>1089</v>
+        <v>1098</v>
       </c>
       <c r="B316" t="s">
-        <v>1090</v>
+        <v>1099</v>
       </c>
       <c r="C316" t="s">
-        <v>1091</v>
+        <v>1100</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -15014,7 +15068,7 @@
         <v>0.95598287878305699</v>
       </c>
       <c r="G316" t="s">
-        <v>1092</v>
+        <v>1101</v>
       </c>
       <c r="H316">
         <v>0.92</v>
@@ -15023,7 +15077,7 @@
         <v>0.97089999999999999</v>
       </c>
       <c r="J316" t="s">
-        <v>1093</v>
+        <v>1102</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -15031,13 +15085,13 @@
     </row>
     <row r="317" spans="1:11">
       <c r="A317" t="s">
-        <v>1094</v>
+        <v>1103</v>
       </c>
       <c r="B317" t="s">
-        <v>1095</v>
+        <v>1104</v>
       </c>
       <c r="C317" t="s">
-        <v>1095</v>
+        <v>1104</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -15066,13 +15120,13 @@
     </row>
     <row r="318" spans="1:11">
       <c r="A318" t="s">
-        <v>1096</v>
+        <v>1105</v>
       </c>
       <c r="B318" t="s">
-        <v>1097</v>
+        <v>1106</v>
       </c>
       <c r="C318" t="s">
-        <v>1098</v>
+        <v>1107</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -15084,7 +15138,7 @@
         <v>0.95178740438847254</v>
       </c>
       <c r="G318" t="s">
-        <v>1099</v>
+        <v>1108</v>
       </c>
       <c r="H318">
         <v>0.9</v>
@@ -15093,7 +15147,7 @@
         <v>0.97430000000000005</v>
       </c>
       <c r="J318" t="s">
-        <v>1100</v>
+        <v>1109</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -15101,13 +15155,13 @@
     </row>
     <row r="319" spans="1:11">
       <c r="A319" t="s">
-        <v>1101</v>
+        <v>1110</v>
       </c>
       <c r="B319" t="s">
-        <v>1102</v>
+        <v>1111</v>
       </c>
       <c r="C319" t="s">
-        <v>1103</v>
+        <v>1112</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -15119,7 +15173,7 @@
         <v>0.70336391437308876</v>
       </c>
       <c r="G319" t="s">
-        <v>1104</v>
+        <v>1113</v>
       </c>
       <c r="H319">
         <v>0.41</v>
@@ -15128,7 +15182,7 @@
         <v>0.80920000000000003</v>
       </c>
       <c r="J319" t="s">
-        <v>1105</v>
+        <v>1114</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -15136,13 +15190,13 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320" t="s">
-        <v>1106</v>
+        <v>1115</v>
       </c>
       <c r="B320" t="s">
-        <v>1107</v>
+        <v>1116</v>
       </c>
       <c r="C320" t="s">
-        <v>1107</v>
+        <v>1116</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -15171,13 +15225,13 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1108</v>
+        <v>1117</v>
       </c>
       <c r="B321" t="s">
-        <v>1109</v>
+        <v>1118</v>
       </c>
       <c r="C321" t="s">
-        <v>1110</v>
+        <v>1119</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -15189,7 +15243,7 @@
         <v>0.99849640734645617</v>
       </c>
       <c r="G321" t="s">
-        <v>1111</v>
+        <v>1120</v>
       </c>
       <c r="H321">
         <v>0.98</v>
@@ -15198,7 +15252,7 @@
         <v>0.99470000000000003</v>
       </c>
       <c r="J321" t="s">
-        <v>1112</v>
+        <v>1121</v>
       </c>
       <c r="K321">
         <v>0</v>
@@ -15206,13 +15260,13 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1113</v>
+        <v>1122</v>
       </c>
       <c r="B322" t="s">
-        <v>1114</v>
+        <v>1123</v>
       </c>
       <c r="C322" t="s">
-        <v>1114</v>
+        <v>1123</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -15241,13 +15295,13 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1115</v>
+        <v>1124</v>
       </c>
       <c r="B323" t="s">
-        <v>1116</v>
+        <v>1125</v>
       </c>
       <c r="C323" t="s">
-        <v>1116</v>
+        <v>1125</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -15276,13 +15330,13 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1117</v>
+        <v>1126</v>
       </c>
       <c r="B324" t="s">
-        <v>1118</v>
+        <v>1127</v>
       </c>
       <c r="C324" t="s">
-        <v>1119</v>
+        <v>1128</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -15294,7 +15348,7 @@
         <v>0.99690437876548454</v>
       </c>
       <c r="G324" t="s">
-        <v>1120</v>
+        <v>1129</v>
       </c>
       <c r="H324">
         <v>0.95</v>
@@ -15303,7 +15357,7 @@
         <v>0.98730000000000007</v>
       </c>
       <c r="J324" t="s">
-        <v>1121</v>
+        <v>1130</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -15311,13 +15365,13 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1122</v>
+        <v>1131</v>
       </c>
       <c r="B325" t="s">
-        <v>1123</v>
+        <v>1132</v>
       </c>
       <c r="C325" t="s">
-        <v>1124</v>
+        <v>1133</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -15329,7 +15383,7 @@
         <v>0.9999968246710359</v>
       </c>
       <c r="G325" t="s">
-        <v>1125</v>
+        <v>1134</v>
       </c>
       <c r="H325">
         <v>1</v>
@@ -15338,7 +15392,7 @@
         <v>1</v>
       </c>
       <c r="J325" t="s">
-        <v>1126</v>
+        <v>1135</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -15346,13 +15400,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1127</v>
+        <v>1136</v>
       </c>
       <c r="B326" t="s">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="C326" t="s">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -15381,13 +15435,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1129</v>
+        <v>1138</v>
       </c>
       <c r="B327" t="s">
-        <v>1130</v>
+        <v>1139</v>
       </c>
       <c r="C327" t="s">
-        <v>1130</v>
+        <v>1139</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Terminate analisi CodeT5_770, modificata presentazione
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/Analisi_CodeT5_770.xlsx
+++ b/HE/W_in_progress/Analisi_CodeT5_770.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28317"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09779C33-FB60-43B1-96AF-33A1928955E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E04A023D-05D4-4F2E-9F0C-BE57DE5BFEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="1150">
   <si>
     <t>IN</t>
   </si>
@@ -3195,6 +3195,9 @@
     <t>0.7407407357597928</t>
   </si>
   <si>
+    <t>Qualche errore, ma ci può stare</t>
+  </si>
+  <si>
     <t>map data_2_o to t_dac_val_2; if bits 21-14 of BAR signal are equal to hexadecimal '2B'; Use the select statement with GPIO_enable signal to determine whether to output data from GPIO_write signal or keep it high impedance (Z).Report an error message with failure severity if the output signal does not equal '0'</t>
   </si>
   <si>
@@ -3210,6 +3213,9 @@
     <t>0.7692307642973374</t>
   </si>
   <si>
+    <t>mancano delle richieste</t>
+  </si>
+  <si>
     <t>declare control as a std_logic_vector signal with 2 bit initialized to all '0'; reg_key_in is an input std_logic_vector of 80 bit</t>
   </si>
   <si>
@@ -3327,6 +3333,9 @@
     <t>0.8727272677289256</t>
   </si>
   <si>
+    <t>Non proprio quello che ho chiesto</t>
+  </si>
+  <si>
     <t>ROM_selector_onboard is an entity with clock_in as input std_logic signal, reset_in as input std_logic signal, addr_strobe_in as input std_logic signal, anodes_out as output std_logic_vector signal of 8 bit, cathodes_out as output std_logic_vector signal of 8 bit; temp_stop_cu ia s std_logic signal; define a signal of type std_logic initialized to 0 and called TbClockA</t>
   </si>
   <si>
@@ -3357,6 +3366,9 @@
     <t>0.9714285664285714</t>
   </si>
   <si>
+    <t>Ho 2 valori in std_logic_vector(1 downto 0) non 1</t>
+  </si>
+  <si>
     <t>if i_start_counter is lesser to START_DLY minus 1, increase i_start_counter signal by 1, set t_start signal to low; using the selected signal assignment, the signal y is set to a0 when signal ciao is low, it is set to a1 when signal ciao is high, otherwise it is set to don't care</t>
   </si>
   <si>
@@ -3391,6 +3403,9 @@
   </si>
   <si>
     <t>0.8148148098765432</t>
+  </si>
+  <si>
+    <t>Ha Fatto altro</t>
   </si>
   <si>
     <t>set signal result_sig as the XOR of input_x and input_y; i_sck_cpy is a signal of type std_logic; pl is an instance of perm_layer component with the signals data_out_temp2, data_out</t>
@@ -3838,8 +3853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C274" workbookViewId="0">
-      <selection activeCell="L302" sqref="L302"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="K328" sqref="K328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14658,18 +14673,21 @@
         <v>1053</v>
       </c>
       <c r="K303">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L303" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="304" spans="1:12">
       <c r="A304" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B304" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C304" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -14681,7 +14699,7 @@
         <v>0.64379423183166962</v>
       </c>
       <c r="G304" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="H304">
         <v>0.56999999999999995</v>
@@ -14690,21 +14708,24 @@
         <v>0.93209999999999993</v>
       </c>
       <c r="J304" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="K304">
         <v>0</v>
       </c>
-    </row>
-    <row r="305" spans="1:11">
+      <c r="L304" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12">
       <c r="A305" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="B305" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C305" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -14731,15 +14752,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:11">
+    <row r="306" spans="1:12">
       <c r="A306" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="B306" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C306" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -14751,7 +14772,7 @@
         <v>0.97417177571210234</v>
       </c>
       <c r="G306" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="H306">
         <v>0.93</v>
@@ -14760,21 +14781,21 @@
         <v>0.98209999999999997</v>
       </c>
       <c r="J306" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="K306">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="307" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12">
       <c r="A307" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="B307" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="C307" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -14801,15 +14822,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:11">
+    <row r="308" spans="1:12">
       <c r="A308" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="B308" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="C308" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -14821,7 +14842,7 @@
         <v>0.98664022774046589</v>
       </c>
       <c r="G308" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="H308">
         <v>0.97</v>
@@ -14830,21 +14851,21 @@
         <v>0.98909999999999998</v>
       </c>
       <c r="J308" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="K308">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12">
       <c r="A309" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="B309" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="C309" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -14856,7 +14877,7 @@
         <v>0.99995890523547304</v>
       </c>
       <c r="G309" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="H309">
         <v>1</v>
@@ -14868,18 +14889,18 @@
         <v>965</v>
       </c>
       <c r="K309">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12">
       <c r="A310" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="B310" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="C310" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -14906,15 +14927,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:11">
+    <row r="311" spans="1:12">
       <c r="A311" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="B311" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="C311" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -14926,7 +14947,7 @@
         <v>0.99998928326474623</v>
       </c>
       <c r="G311" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="H311">
         <v>1</v>
@@ -14938,18 +14959,18 @@
         <v>107</v>
       </c>
       <c r="K311">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12">
       <c r="A312" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="B312" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="C312" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -14961,7 +14982,7 @@
         <v>0.97341886358453711</v>
       </c>
       <c r="G312" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="H312">
         <v>0.94</v>
@@ -14970,21 +14991,21 @@
         <v>0.97719999999999996</v>
       </c>
       <c r="J312" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="K312">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12">
       <c r="A313" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="B313" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="C313" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -14996,7 +15017,7 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="H313">
         <v>0.89</v>
@@ -15005,21 +15026,21 @@
         <v>0.9756999999999999</v>
       </c>
       <c r="J313" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="K313">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12">
       <c r="A314" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="B314" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="C314" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -15031,7 +15052,7 @@
         <v>0.75858170895276666</v>
       </c>
       <c r="G314" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="H314">
         <v>0.54</v>
@@ -15040,21 +15061,24 @@
         <v>0.68030000000000002</v>
       </c>
       <c r="J314" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="K314">
         <v>0</v>
       </c>
-    </row>
-    <row r="315" spans="1:11">
+      <c r="L314" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12">
       <c r="A315" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="B315" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="C315" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -15066,7 +15090,7 @@
         <v>0.998317618783509</v>
       </c>
       <c r="G315" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="H315">
         <v>0.9</v>
@@ -15075,21 +15099,21 @@
         <v>0.97470000000000001</v>
       </c>
       <c r="J315" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="K315">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12">
       <c r="A316" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
       <c r="B316" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="C316" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -15101,7 +15125,7 @@
         <v>0.95598287878305699</v>
       </c>
       <c r="G316" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="H316">
         <v>0.92</v>
@@ -15110,21 +15134,24 @@
         <v>0.97089999999999999</v>
       </c>
       <c r="J316" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="K316">
         <v>0</v>
       </c>
-    </row>
-    <row r="317" spans="1:11">
+      <c r="L316" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12">
       <c r="A317" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="B317" t="s">
-        <v>1109</v>
+        <v>1113</v>
       </c>
       <c r="C317" t="s">
-        <v>1109</v>
+        <v>1113</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -15151,15 +15178,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:11">
+    <row r="318" spans="1:12">
       <c r="A318" t="s">
-        <v>1110</v>
+        <v>1114</v>
       </c>
       <c r="B318" t="s">
-        <v>1111</v>
+        <v>1115</v>
       </c>
       <c r="C318" t="s">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -15171,7 +15198,7 @@
         <v>0.95178740438847254</v>
       </c>
       <c r="G318" t="s">
-        <v>1113</v>
+        <v>1117</v>
       </c>
       <c r="H318">
         <v>0.9</v>
@@ -15180,21 +15207,21 @@
         <v>0.97430000000000005</v>
       </c>
       <c r="J318" t="s">
-        <v>1114</v>
+        <v>1118</v>
       </c>
       <c r="K318">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12">
       <c r="A319" t="s">
-        <v>1115</v>
+        <v>1119</v>
       </c>
       <c r="B319" t="s">
-        <v>1116</v>
+        <v>1120</v>
       </c>
       <c r="C319" t="s">
-        <v>1117</v>
+        <v>1121</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -15206,7 +15233,7 @@
         <v>0.70336391437308876</v>
       </c>
       <c r="G319" t="s">
-        <v>1118</v>
+        <v>1122</v>
       </c>
       <c r="H319">
         <v>0.41</v>
@@ -15215,21 +15242,24 @@
         <v>0.80920000000000003</v>
       </c>
       <c r="J319" t="s">
-        <v>1119</v>
+        <v>1123</v>
       </c>
       <c r="K319">
         <v>0</v>
       </c>
-    </row>
-    <row r="320" spans="1:11">
+      <c r="L319" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12">
       <c r="A320" t="s">
-        <v>1120</v>
+        <v>1125</v>
       </c>
       <c r="B320" t="s">
-        <v>1121</v>
+        <v>1126</v>
       </c>
       <c r="C320" t="s">
-        <v>1121</v>
+        <v>1126</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -15258,13 +15288,13 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321" t="s">
-        <v>1122</v>
+        <v>1127</v>
       </c>
       <c r="B321" t="s">
-        <v>1123</v>
+        <v>1128</v>
       </c>
       <c r="C321" t="s">
-        <v>1124</v>
+        <v>1129</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -15276,7 +15306,7 @@
         <v>0.99849640734645617</v>
       </c>
       <c r="G321" t="s">
-        <v>1125</v>
+        <v>1130</v>
       </c>
       <c r="H321">
         <v>0.98</v>
@@ -15285,21 +15315,21 @@
         <v>0.99470000000000003</v>
       </c>
       <c r="J321" t="s">
-        <v>1126</v>
+        <v>1131</v>
       </c>
       <c r="K321">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="322" spans="1:11">
       <c r="A322" t="s">
-        <v>1127</v>
+        <v>1132</v>
       </c>
       <c r="B322" t="s">
-        <v>1128</v>
+        <v>1133</v>
       </c>
       <c r="C322" t="s">
-        <v>1128</v>
+        <v>1133</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -15328,13 +15358,13 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323" t="s">
-        <v>1129</v>
+        <v>1134</v>
       </c>
       <c r="B323" t="s">
-        <v>1130</v>
+        <v>1135</v>
       </c>
       <c r="C323" t="s">
-        <v>1130</v>
+        <v>1135</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -15363,13 +15393,13 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" t="s">
-        <v>1131</v>
+        <v>1136</v>
       </c>
       <c r="B324" t="s">
-        <v>1132</v>
+        <v>1137</v>
       </c>
       <c r="C324" t="s">
-        <v>1133</v>
+        <v>1138</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -15381,7 +15411,7 @@
         <v>0.99690437876548454</v>
       </c>
       <c r="G324" t="s">
-        <v>1134</v>
+        <v>1139</v>
       </c>
       <c r="H324">
         <v>0.95</v>
@@ -15390,21 +15420,21 @@
         <v>0.98730000000000007</v>
       </c>
       <c r="J324" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="K324">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:11">
       <c r="A325" t="s">
-        <v>1136</v>
+        <v>1141</v>
       </c>
       <c r="B325" t="s">
-        <v>1137</v>
+        <v>1142</v>
       </c>
       <c r="C325" t="s">
-        <v>1138</v>
+        <v>1143</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -15416,7 +15446,7 @@
         <v>0.9999968246710359</v>
       </c>
       <c r="G325" t="s">
-        <v>1139</v>
+        <v>1144</v>
       </c>
       <c r="H325">
         <v>1</v>
@@ -15425,7 +15455,7 @@
         <v>1</v>
       </c>
       <c r="J325" t="s">
-        <v>1140</v>
+        <v>1145</v>
       </c>
       <c r="K325">
         <v>1</v>
@@ -15433,13 +15463,13 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" t="s">
-        <v>1141</v>
+        <v>1146</v>
       </c>
       <c r="B326" t="s">
-        <v>1142</v>
+        <v>1147</v>
       </c>
       <c r="C326" t="s">
-        <v>1142</v>
+        <v>1147</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -15468,13 +15498,13 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" t="s">
-        <v>1143</v>
+        <v>1148</v>
       </c>
       <c r="B327" t="s">
-        <v>1144</v>
+        <v>1149</v>
       </c>
       <c r="C327" t="s">
-        <v>1144</v>
+        <v>1149</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>